<commit_message>
Various bug fixes; new TB output to use commas instead of newlines
</commit_message>
<xml_diff>
--- a/assay_data/TB_assays.xlsx
+++ b/assay_data/TB_assays.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="140">
   <si>
     <t>Assay Name</t>
   </si>
@@ -446,6 +446,21 @@
   </si>
   <si>
     <t>rrs 1484 mutation present which is associated with capreomycin and amikacin resistance.</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>embB</t>
+  </si>
+  <si>
+    <t>GCTGATTCCGGCAAGCTGGCGCACCTTCACCCTGACCGACGCCGTGGTGATATTCGGCTTCCTGCTCTGGCATGTCATCGGCGCGAATTCGTCGGACGACGGCTACATCCTGGGCATGGCCCGAGTCGCCGACCACGCCGGCTACATGTCCAACTATTTCCGCTGGTTCGGCAGCCCGGAGGATCCCTTCGGCTGGTATTACAACCTGCTGGCGCTGATGACCCATGTCAGCGACGCCAGTCTGTGGATGCGCCTGCCAGACCTGGCCGCCGGGCTAGTGTGCTGGCTGCTGCTGTCGCGTGAGGTGCTGCCCCGCCTCGGGCCGGCGGTGGAGGCCAGCAAACCCGCCTACTGGGCGGCGGCCATGGTCTTGCTGACCGCGTGGATGCCGTTCAACAACGGCCTGCGGCCGGAGGGCATCATCGCGCTCGGCTCGCTGGTCACCTATGT</t>
+  </si>
+  <si>
+    <t>embB mutation present which may be associated with ethambutal resistance</t>
+  </si>
+  <si>
+    <t>Ethambutal</t>
   </si>
 </sst>
 </file>
@@ -1788,10 +1803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG707"/>
+  <dimension ref="A1:AG708"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2102,6 +2117,9 @@
       <c r="D8" t="s">
         <v>51</v>
       </c>
+      <c r="G8" t="s">
+        <v>135</v>
+      </c>
       <c r="I8" s="8" t="s">
         <v>52</v>
       </c>
@@ -2213,143 +2231,153 @@
     </row>
     <row r="13" spans="1:33">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="J13" s="35"/>
+      <c r="K13" s="36">
+        <v>0</v>
+      </c>
+      <c r="L13" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="M13" s="36"/>
+      <c r="R13" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="S13" s="31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33">
+      <c r="A14" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="N13">
+      <c r="N14">
         <v>88</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O14" t="s">
         <v>60</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P14" t="s">
         <v>61</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="Q14" t="s">
         <v>62</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R14" t="s">
         <v>63</v>
-      </c>
-      <c r="S13" s="31" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33">
-      <c r="D14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="N14">
-        <v>90</v>
-      </c>
-      <c r="O14" t="s">
-        <v>65</v>
-      </c>
-      <c r="P14" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>67</v>
-      </c>
-      <c r="R14" t="s">
-        <v>68</v>
       </c>
       <c r="S14" s="31" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:33">
+      <c r="D15" s="8"/>
       <c r="I15" s="8"/>
       <c r="N15">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O15" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="P15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="Q15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="R15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S15" s="31" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:33">
-      <c r="D16" s="8"/>
       <c r="I16" s="8"/>
       <c r="N16">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="O16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="P16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="Q16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="R16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S16" s="31" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" t="s">
+      <c r="D17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="N17">
+        <v>94</v>
+      </c>
+      <c r="O17" t="s">
+        <v>74</v>
+      </c>
+      <c r="P17" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>76</v>
+      </c>
+      <c r="R17" t="s">
+        <v>70</v>
+      </c>
+      <c r="S17" s="31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" t="s">
         <v>77</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>25</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>77</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I18" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="J17" s="35" t="s">
+      <c r="J18" s="35" t="s">
         <v>79</v>
-      </c>
-      <c r="K17" s="28">
-        <v>1150</v>
-      </c>
-      <c r="L17" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="M17" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="R17" t="s">
-        <v>98</v>
-      </c>
-      <c r="S17" s="31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19">
-      <c r="I18" s="8"/>
-      <c r="J18" s="35" t="s">
-        <v>80</v>
       </c>
       <c r="K18" s="28">
         <v>1150</v>
@@ -2358,7 +2386,7 @@
         <v>46</v>
       </c>
       <c r="M18" s="28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R18" t="s">
         <v>98</v>
@@ -2370,7 +2398,7 @@
     <row r="19" spans="1:19">
       <c r="I19" s="8"/>
       <c r="J19" s="35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K19" s="28">
         <v>1150</v>
@@ -2379,7 +2407,7 @@
         <v>46</v>
       </c>
       <c r="M19" s="28" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="R19" t="s">
         <v>98</v>
@@ -2391,19 +2419,19 @@
     <row r="20" spans="1:19">
       <c r="I20" s="8"/>
       <c r="J20" s="35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K20" s="28">
-        <v>1143</v>
+        <v>1150</v>
       </c>
       <c r="L20" s="28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M20" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S20" s="31" t="s">
         <v>47</v>
@@ -2412,54 +2440,40 @@
     <row r="21" spans="1:19">
       <c r="I21" s="8"/>
       <c r="J21" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K21" s="28">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="L21" s="28" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="M21" s="28" t="s">
         <v>46</v>
       </c>
       <c r="R21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S21" s="31" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" t="s">
-        <v>84</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="N22">
-        <v>315</v>
-      </c>
-      <c r="O22" t="s">
-        <v>86</v>
-      </c>
-      <c r="P22" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>88</v>
+      <c r="I22" s="8"/>
+      <c r="J22" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="K22" s="28">
+        <v>1141</v>
+      </c>
+      <c r="L22" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="M22" s="28" t="s">
+        <v>46</v>
       </c>
       <c r="R22" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="S22" s="31" t="s">
         <v>47</v>
@@ -2467,7 +2481,7 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
@@ -2476,46 +2490,63 @@
         <v>25</v>
       </c>
       <c r="D23" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" t="s">
+        <v>135</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="N23">
+        <v>315</v>
+      </c>
+      <c r="O23" t="s">
+        <v>86</v>
+      </c>
+      <c r="P23" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>88</v>
+      </c>
+      <c r="R23" t="s">
+        <v>89</v>
+      </c>
+      <c r="S23" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" t="s">
         <v>101</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="N23">
+      <c r="N24">
         <v>513</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O24" t="s">
         <v>103</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P24" t="s">
         <v>104</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="Q24" t="s">
         <v>105</v>
       </c>
-      <c r="R23" t="s">
+      <c r="R24" t="s">
         <v>106</v>
-      </c>
-      <c r="S23" s="31" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19">
-      <c r="I24" s="8"/>
-      <c r="N24">
-        <v>516</v>
-      </c>
-      <c r="O24" t="s">
-        <v>108</v>
-      </c>
-      <c r="P24" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>114</v>
-      </c>
-      <c r="R24" t="s">
-        <v>109</v>
       </c>
       <c r="S24" s="31" t="s">
         <v>107</v>
@@ -2524,19 +2555,19 @@
     <row r="25" spans="1:19">
       <c r="I25" s="8"/>
       <c r="N25">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="O25" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="P25" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="Q25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S25" s="31" t="s">
         <v>107</v>
@@ -2545,19 +2576,19 @@
     <row r="26" spans="1:19">
       <c r="I26" s="8"/>
       <c r="N26">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="O26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P26" t="s">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="Q26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="R26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S26" s="31" t="s">
         <v>107</v>
@@ -2566,19 +2597,19 @@
     <row r="27" spans="1:19">
       <c r="I27" s="8"/>
       <c r="N27">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="O27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="P27" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="Q27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="R27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S27" s="31" t="s">
         <v>107</v>
@@ -2587,104 +2618,121 @@
     <row r="28" spans="1:19">
       <c r="I28" s="8"/>
       <c r="N28">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="O28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P28" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="Q28" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="R28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S28" s="31" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" t="s">
+      <c r="I29" s="8"/>
+      <c r="N29">
+        <v>533</v>
+      </c>
+      <c r="O29" t="s">
+        <v>122</v>
+      </c>
+      <c r="P29" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>73</v>
+      </c>
+      <c r="R29" t="s">
+        <v>113</v>
+      </c>
+      <c r="S29" s="31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" t="s">
         <v>124</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>20</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>25</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>124</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I30" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="J29" s="28" t="s">
+      <c r="J30" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="K29" s="28">
+      <c r="K30" s="28">
         <v>1063</v>
       </c>
-      <c r="L29" s="28" t="s">
+      <c r="L30" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="M29" s="28" t="s">
+      <c r="M30" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="R29" t="s">
+      <c r="R30" t="s">
         <v>127</v>
       </c>
-      <c r="S29" s="31" t="s">
+      <c r="S30" s="31" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19">
-      <c r="I30" s="8"/>
-      <c r="J30" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="K30" s="28">
-        <v>1064</v>
-      </c>
-      <c r="L30" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="M30" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="R30" t="s">
-        <v>133</v>
-      </c>
-      <c r="S30" s="31" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:19">
       <c r="I31" s="8"/>
       <c r="J31" s="28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K31" s="28">
-        <v>1146</v>
+        <v>1064</v>
       </c>
       <c r="L31" s="28" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="M31" s="28" t="s">
         <v>46</v>
       </c>
       <c r="R31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S31" s="31" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:19">
       <c r="I32" s="8"/>
-      <c r="S32" s="31"/>
+      <c r="J32" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="K32" s="28">
+        <v>1146</v>
+      </c>
+      <c r="L32" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="M32" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="R32" t="s">
+        <v>134</v>
+      </c>
+      <c r="S32" s="31" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="33" spans="9:19">
       <c r="I33" s="8"/>
@@ -2759,7 +2807,6 @@
       <c r="S50" s="31"/>
     </row>
     <row r="51" spans="4:19">
-      <c r="D51" s="8"/>
       <c r="I51" s="8"/>
       <c r="S51" s="31"/>
     </row>
@@ -2769,6 +2816,7 @@
       <c r="S52" s="31"/>
     </row>
     <row r="53" spans="4:19">
+      <c r="D53" s="8"/>
       <c r="I53" s="8"/>
       <c r="S53" s="31"/>
     </row>
@@ -2777,7 +2825,6 @@
       <c r="S54" s="31"/>
     </row>
     <row r="55" spans="4:19">
-      <c r="D55" s="8"/>
       <c r="I55" s="8"/>
       <c r="S55" s="31"/>
     </row>
@@ -2794,11 +2841,12 @@
     <row r="58" spans="4:19">
       <c r="D58" s="8"/>
       <c r="I58" s="8"/>
-      <c r="R58" s="21"/>
       <c r="S58" s="31"/>
     </row>
     <row r="59" spans="4:19">
+      <c r="D59" s="8"/>
       <c r="I59" s="8"/>
+      <c r="R59" s="21"/>
       <c r="S59" s="31"/>
     </row>
     <row r="60" spans="4:19">
@@ -2831,7 +2879,6 @@
     </row>
     <row r="67" spans="4:20">
       <c r="I67" s="8"/>
-      <c r="R67" s="21"/>
       <c r="S67" s="31"/>
     </row>
     <row r="68" spans="4:20">
@@ -2840,17 +2887,18 @@
       <c r="S68" s="31"/>
     </row>
     <row r="69" spans="4:20">
-      <c r="D69" s="8"/>
       <c r="I69" s="8"/>
+      <c r="R69" s="21"/>
       <c r="S69" s="31"/>
-      <c r="T69" s="14"/>
     </row>
     <row r="70" spans="4:20">
       <c r="D70" s="8"/>
       <c r="I70" s="8"/>
       <c r="S70" s="31"/>
+      <c r="T70" s="14"/>
     </row>
     <row r="71" spans="4:20">
+      <c r="D71" s="8"/>
       <c r="I71" s="8"/>
       <c r="S71" s="31"/>
     </row>
@@ -2880,7 +2928,6 @@
     </row>
     <row r="78" spans="4:20">
       <c r="I78" s="8"/>
-      <c r="R78" s="22"/>
       <c r="S78" s="31"/>
     </row>
     <row r="79" spans="4:20">
@@ -2889,8 +2936,8 @@
       <c r="S79" s="31"/>
     </row>
     <row r="80" spans="4:20">
-      <c r="D80" s="8"/>
       <c r="I80" s="8"/>
+      <c r="R80" s="22"/>
       <c r="S80" s="31"/>
     </row>
     <row r="81" spans="1:32">
@@ -2899,51 +2946,51 @@
       <c r="S81" s="31"/>
     </row>
     <row r="82" spans="1:32">
+      <c r="D82" s="8"/>
       <c r="I82" s="8"/>
-      <c r="R82" s="5"/>
       <c r="S82" s="31"/>
-      <c r="AD82" s="6"/>
-      <c r="AE82" s="7"/>
-      <c r="AF82" s="5"/>
     </row>
     <row r="83" spans="1:32">
-      <c r="A83" s="16"/>
-      <c r="B83" s="17"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="18"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5"/>
-      <c r="H83" s="5"/>
-      <c r="I83" s="20"/>
-      <c r="J83" s="30"/>
-      <c r="K83" s="27"/>
-      <c r="L83" s="27"/>
-      <c r="M83" s="27"/>
-      <c r="N83" s="5"/>
-      <c r="O83" s="5"/>
-      <c r="P83" s="5"/>
-      <c r="Q83" s="5"/>
+      <c r="I83" s="8"/>
       <c r="R83" s="5"/>
-      <c r="S83" s="32"/>
-      <c r="T83" s="5"/>
-      <c r="U83" s="5"/>
-      <c r="V83" s="5"/>
-      <c r="W83" s="5"/>
-      <c r="X83" s="5"/>
-      <c r="Y83" s="5"/>
-      <c r="Z83" s="5"/>
-      <c r="AA83" s="5"/>
-      <c r="AB83" s="5"/>
-      <c r="AC83" s="5"/>
+      <c r="S83" s="31"/>
       <c r="AD83" s="6"/>
       <c r="AE83" s="7"/>
       <c r="AF83" s="5"/>
     </row>
     <row r="84" spans="1:32">
-      <c r="I84" s="8"/>
+      <c r="A84" s="16"/>
+      <c r="B84" s="17"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="20"/>
+      <c r="J84" s="30"/>
+      <c r="K84" s="27"/>
+      <c r="L84" s="27"/>
+      <c r="M84" s="27"/>
+      <c r="N84" s="5"/>
+      <c r="O84" s="5"/>
+      <c r="P84" s="5"/>
+      <c r="Q84" s="5"/>
       <c r="R84" s="5"/>
-      <c r="S84" s="31"/>
+      <c r="S84" s="32"/>
+      <c r="T84" s="5"/>
+      <c r="U84" s="5"/>
+      <c r="V84" s="5"/>
+      <c r="W84" s="5"/>
+      <c r="X84" s="5"/>
+      <c r="Y84" s="5"/>
+      <c r="Z84" s="5"/>
+      <c r="AA84" s="5"/>
+      <c r="AB84" s="5"/>
+      <c r="AC84" s="5"/>
+      <c r="AD84" s="6"/>
+      <c r="AE84" s="7"/>
+      <c r="AF84" s="5"/>
     </row>
     <row r="85" spans="1:32">
       <c r="I85" s="8"/>
@@ -2952,6 +2999,7 @@
     </row>
     <row r="86" spans="1:32">
       <c r="I86" s="8"/>
+      <c r="R86" s="5"/>
       <c r="S86" s="31"/>
     </row>
     <row r="87" spans="1:32">
@@ -2963,14 +3011,14 @@
       <c r="S88" s="31"/>
     </row>
     <row r="89" spans="1:32">
-      <c r="D89" s="8"/>
       <c r="I89" s="8"/>
       <c r="S89" s="31"/>
-      <c r="T89" s="14"/>
     </row>
     <row r="90" spans="1:32">
+      <c r="D90" s="8"/>
       <c r="I90" s="8"/>
       <c r="S90" s="31"/>
+      <c r="T90" s="14"/>
     </row>
     <row r="91" spans="1:32">
       <c r="I91" s="8"/>
@@ -3009,22 +3057,22 @@
       <c r="S99" s="31"/>
     </row>
     <row r="100" spans="4:19">
-      <c r="D100" s="8"/>
-      <c r="I100" s="10"/>
-      <c r="J100" s="29"/>
-      <c r="S100" s="32"/>
+      <c r="I100" s="8"/>
+      <c r="S100" s="31"/>
     </row>
     <row r="101" spans="4:19">
-      <c r="I101" s="8"/>
-      <c r="R101" s="22"/>
-      <c r="S101" s="33"/>
+      <c r="D101" s="8"/>
+      <c r="I101" s="10"/>
+      <c r="J101" s="29"/>
+      <c r="S101" s="32"/>
     </row>
     <row r="102" spans="4:19">
-      <c r="D102" s="8"/>
       <c r="I102" s="8"/>
-      <c r="S102" s="31"/>
+      <c r="R102" s="22"/>
+      <c r="S102" s="33"/>
     </row>
     <row r="103" spans="4:19">
+      <c r="D103" s="8"/>
       <c r="I103" s="8"/>
       <c r="S103" s="31"/>
     </row>
@@ -3061,7 +3109,6 @@
       <c r="S111" s="31"/>
     </row>
     <row r="112" spans="4:19">
-      <c r="D112" s="8"/>
       <c r="I112" s="8"/>
       <c r="S112" s="31"/>
     </row>
@@ -3081,8 +3128,9 @@
       <c r="S115" s="31"/>
     </row>
     <row r="116" spans="4:19">
+      <c r="D116" s="8"/>
       <c r="I116" s="8"/>
-      <c r="S116" s="34"/>
+      <c r="S116" s="31"/>
     </row>
     <row r="117" spans="4:19">
       <c r="I117" s="8"/>
@@ -3090,11 +3138,11 @@
     </row>
     <row r="118" spans="4:19">
       <c r="I118" s="8"/>
-      <c r="S118" s="32"/>
+      <c r="S118" s="34"/>
     </row>
     <row r="119" spans="4:19">
       <c r="I119" s="8"/>
-      <c r="S119" s="31"/>
+      <c r="S119" s="32"/>
     </row>
     <row r="120" spans="4:19">
       <c r="I120" s="8"/>
@@ -3102,7 +3150,7 @@
     </row>
     <row r="121" spans="4:19">
       <c r="I121" s="8"/>
-      <c r="S121" s="32"/>
+      <c r="S121" s="31"/>
     </row>
     <row r="122" spans="4:19">
       <c r="I122" s="8"/>
@@ -3113,17 +3161,16 @@
       <c r="S123" s="32"/>
     </row>
     <row r="124" spans="4:19">
-      <c r="R124" s="22"/>
-      <c r="S124" s="33"/>
+      <c r="I124" s="8"/>
+      <c r="S124" s="32"/>
     </row>
     <row r="125" spans="4:19">
       <c r="R125" s="22"/>
       <c r="S125" s="33"/>
     </row>
     <row r="126" spans="4:19">
-      <c r="D126" s="8"/>
-      <c r="I126" s="8"/>
-      <c r="S126" s="34"/>
+      <c r="R126" s="22"/>
+      <c r="S126" s="33"/>
     </row>
     <row r="127" spans="4:19">
       <c r="D127" s="8"/>
@@ -3132,9 +3179,8 @@
     </row>
     <row r="128" spans="4:19">
       <c r="D128" s="8"/>
-      <c r="I128" s="10"/>
-      <c r="J128" s="29"/>
-      <c r="S128" s="32"/>
+      <c r="I128" s="8"/>
+      <c r="S128" s="34"/>
     </row>
     <row r="129" spans="4:19">
       <c r="D129" s="8"/>
@@ -3144,8 +3190,9 @@
     </row>
     <row r="130" spans="4:19">
       <c r="D130" s="8"/>
-      <c r="I130" s="8"/>
-      <c r="S130" s="31"/>
+      <c r="I130" s="10"/>
+      <c r="J130" s="29"/>
+      <c r="S130" s="32"/>
     </row>
     <row r="131" spans="4:19">
       <c r="D131" s="8"/>
@@ -3163,6 +3210,7 @@
       <c r="S133" s="31"/>
     </row>
     <row r="134" spans="4:19">
+      <c r="D134" s="8"/>
       <c r="I134" s="8"/>
       <c r="S134" s="31"/>
     </row>
@@ -3184,7 +3232,6 @@
     </row>
     <row r="139" spans="4:19">
       <c r="I139" s="8"/>
-      <c r="R139" s="11"/>
       <c r="S139" s="31"/>
     </row>
     <row r="140" spans="4:19">
@@ -3208,8 +3255,8 @@
       <c r="S143" s="31"/>
     </row>
     <row r="144" spans="4:19">
-      <c r="D144" s="8"/>
       <c r="I144" s="8"/>
+      <c r="R144" s="11"/>
       <c r="S144" s="31"/>
     </row>
     <row r="145" spans="4:20">
@@ -3218,8 +3265,8 @@
       <c r="S145" s="31"/>
     </row>
     <row r="146" spans="4:20">
+      <c r="D146" s="8"/>
       <c r="I146" s="8"/>
-      <c r="R146" s="12"/>
       <c r="S146" s="31"/>
     </row>
     <row r="147" spans="4:20">
@@ -3228,8 +3275,8 @@
       <c r="S147" s="31"/>
     </row>
     <row r="148" spans="4:20">
-      <c r="D148" s="8"/>
       <c r="I148" s="8"/>
+      <c r="R148" s="12"/>
       <c r="S148" s="31"/>
     </row>
     <row r="149" spans="4:20">
@@ -3256,21 +3303,22 @@
       <c r="D153" s="8"/>
       <c r="I153" s="8"/>
       <c r="S153" s="31"/>
-      <c r="T153" s="14"/>
     </row>
     <row r="154" spans="4:20">
       <c r="D154" s="8"/>
       <c r="I154" s="8"/>
       <c r="S154" s="31"/>
+      <c r="T154" s="14"/>
     </row>
     <row r="155" spans="4:20">
       <c r="D155" s="8"/>
       <c r="I155" s="8"/>
-      <c r="R155" s="21"/>
       <c r="S155" s="31"/>
     </row>
     <row r="156" spans="4:20">
+      <c r="D156" s="8"/>
       <c r="I156" s="8"/>
+      <c r="R156" s="21"/>
       <c r="S156" s="31"/>
     </row>
     <row r="157" spans="4:20">
@@ -3311,125 +3359,126 @@
     </row>
     <row r="166" spans="1:32">
       <c r="I166" s="8"/>
-      <c r="R166" s="22"/>
       <c r="S166" s="31"/>
     </row>
     <row r="167" spans="1:32">
-      <c r="D167" s="8"/>
       <c r="I167" s="8"/>
+      <c r="R167" s="22"/>
       <c r="S167" s="31"/>
     </row>
-    <row r="168" spans="1:32" s="13" customFormat="1">
-      <c r="A168"/>
-      <c r="B168"/>
-      <c r="C168"/>
-      <c r="D168"/>
-      <c r="E168"/>
-      <c r="F168"/>
-      <c r="G168"/>
-      <c r="H168"/>
-      <c r="I168"/>
-      <c r="J168" s="28"/>
-      <c r="K168" s="28"/>
-      <c r="L168" s="28"/>
-      <c r="M168" s="28"/>
-      <c r="N168"/>
-      <c r="O168"/>
-      <c r="P168"/>
-      <c r="Q168"/>
-      <c r="R168"/>
+    <row r="168" spans="1:32">
+      <c r="D168" s="8"/>
+      <c r="I168" s="8"/>
       <c r="S168" s="31"/>
-      <c r="T168"/>
-      <c r="U168"/>
-      <c r="V168"/>
-      <c r="W168"/>
-      <c r="X168"/>
-      <c r="Y168"/>
-      <c r="Z168"/>
-      <c r="AA168"/>
-      <c r="AB168"/>
-      <c r="AC168"/>
-      <c r="AD168"/>
-      <c r="AE168"/>
-      <c r="AF168"/>
-    </row>
-    <row r="169" spans="1:32">
+    </row>
+    <row r="169" spans="1:32" s="13" customFormat="1">
+      <c r="A169"/>
+      <c r="B169"/>
+      <c r="C169"/>
+      <c r="D169"/>
+      <c r="E169"/>
+      <c r="F169"/>
+      <c r="G169"/>
+      <c r="H169"/>
+      <c r="I169"/>
+      <c r="J169" s="28"/>
+      <c r="K169" s="28"/>
+      <c r="L169" s="28"/>
+      <c r="M169" s="28"/>
+      <c r="N169"/>
+      <c r="O169"/>
+      <c r="P169"/>
+      <c r="Q169"/>
+      <c r="R169"/>
       <c r="S169" s="31"/>
+      <c r="T169"/>
+      <c r="U169"/>
+      <c r="V169"/>
+      <c r="W169"/>
+      <c r="X169"/>
+      <c r="Y169"/>
+      <c r="Z169"/>
+      <c r="AA169"/>
+      <c r="AB169"/>
+      <c r="AC169"/>
+      <c r="AD169"/>
+      <c r="AE169"/>
+      <c r="AF169"/>
     </row>
     <row r="170" spans="1:32">
-      <c r="I170" s="8"/>
-      <c r="R170" s="21"/>
       <c r="S170" s="31"/>
     </row>
     <row r="171" spans="1:32">
-      <c r="D171" s="8"/>
+      <c r="I171" s="8"/>
+      <c r="R171" s="21"/>
       <c r="S171" s="31"/>
     </row>
     <row r="172" spans="1:32">
+      <c r="D172" s="8"/>
       <c r="S172" s="31"/>
     </row>
     <row r="173" spans="1:32">
       <c r="S173" s="31"/>
     </row>
     <row r="174" spans="1:32">
-      <c r="D174" s="8"/>
-      <c r="I174" s="8"/>
       <c r="S174" s="31"/>
     </row>
     <row r="175" spans="1:32">
+      <c r="D175" s="8"/>
       <c r="I175" s="8"/>
       <c r="S175" s="31"/>
     </row>
     <row r="176" spans="1:32">
-      <c r="D176" s="8"/>
+      <c r="I176" s="8"/>
       <c r="S176" s="31"/>
     </row>
-    <row r="177" spans="19:19">
+    <row r="177" spans="4:19">
+      <c r="D177" s="8"/>
       <c r="S177" s="31"/>
     </row>
-    <row r="178" spans="19:19">
+    <row r="178" spans="4:19">
       <c r="S178" s="31"/>
     </row>
-    <row r="179" spans="19:19">
+    <row r="179" spans="4:19">
       <c r="S179" s="31"/>
     </row>
-    <row r="180" spans="19:19">
+    <row r="180" spans="4:19">
       <c r="S180" s="31"/>
     </row>
-    <row r="181" spans="19:19">
+    <row r="181" spans="4:19">
       <c r="S181" s="31"/>
     </row>
-    <row r="182" spans="19:19">
+    <row r="182" spans="4:19">
       <c r="S182" s="31"/>
     </row>
-    <row r="183" spans="19:19">
+    <row r="183" spans="4:19">
       <c r="S183" s="31"/>
     </row>
-    <row r="184" spans="19:19">
+    <row r="184" spans="4:19">
       <c r="S184" s="31"/>
     </row>
-    <row r="185" spans="19:19">
+    <row r="185" spans="4:19">
       <c r="S185" s="31"/>
     </row>
-    <row r="186" spans="19:19">
+    <row r="186" spans="4:19">
       <c r="S186" s="31"/>
     </row>
-    <row r="187" spans="19:19">
+    <row r="187" spans="4:19">
       <c r="S187" s="31"/>
     </row>
-    <row r="188" spans="19:19">
+    <row r="188" spans="4:19">
       <c r="S188" s="31"/>
     </row>
-    <row r="189" spans="19:19">
+    <row r="189" spans="4:19">
       <c r="S189" s="31"/>
     </row>
-    <row r="190" spans="19:19">
+    <row r="190" spans="4:19">
       <c r="S190" s="31"/>
     </row>
-    <row r="191" spans="19:19">
+    <row r="191" spans="4:19">
       <c r="S191" s="31"/>
     </row>
-    <row r="192" spans="19:19">
+    <row r="192" spans="4:19">
       <c r="S192" s="31"/>
     </row>
     <row r="193" spans="19:19">
@@ -4976,6 +5025,9 @@
     </row>
     <row r="707" spans="19:19">
       <c r="S707" s="31"/>
+    </row>
+    <row r="708" spans="19:19">
+      <c r="S708" s="31"/>
     </row>
   </sheetData>
   <sortState ref="A3:AD178">
@@ -4990,10 +5042,10 @@
     <mergeCell ref="J1:M1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B302">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B303">
       <formula1>$AD$1:$AG$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C302">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C303">
       <formula1>$AD$2:$AG$2</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update to TB_WHO json for consistency and to fix issue that caused a missing mutation
</commit_message>
<xml_diff>
--- a/assay_data/TB_assays.xlsx
+++ b/assay_data/TB_assays.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="2060" windowWidth="39580" windowHeight="23100" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21960" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TB" sheetId="1" r:id="rId1"/>
@@ -117,7 +117,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
       <t>/NT</t>
@@ -128,7 +127,6 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> Sequence</t>
@@ -1778,12 +1776,6 @@
     <t>7581-7583</t>
   </si>
   <si>
-    <t>A504V</t>
-  </si>
-  <si>
-    <t>E459K</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -2706,6 +2698,12 @@
   <si>
     <t>references/ASM19595v2.fasta</t>
   </si>
+  <si>
+    <t>E459</t>
+  </si>
+  <si>
+    <t>A504</t>
+  </si>
 </sst>
 </file>
 
@@ -2717,7 +2715,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3568,6 +3565,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3603,12 +3606,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="449">
@@ -4419,37 +4416,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="1" customFormat="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="69" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="68" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="68"/>
-      <c r="J1" s="69" t="s">
+      <c r="I1" s="70"/>
+      <c r="J1" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="69" t="s">
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="66" t="s">
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="67"/>
+      <c r="S1" s="69"/>
       <c r="AD1" s="23" t="s">
         <v>19</v>
       </c>
@@ -9712,37 +9709,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="1" customFormat="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="69" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="68" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="68"/>
-      <c r="J1" s="69" t="s">
+      <c r="I1" s="70"/>
+      <c r="J1" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="69" t="s">
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="66" t="s">
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="67"/>
+      <c r="S1" s="69"/>
       <c r="AD1" s="23" t="s">
         <v>19</v>
       </c>
@@ -15057,37 +15054,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="38" customFormat="1">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="75" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="74" t="s">
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="74"/>
-      <c r="J1" s="75" t="s">
+      <c r="I1" s="76"/>
+      <c r="J1" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="75" t="s">
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="72" t="s">
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="73"/>
+      <c r="S1" s="75"/>
       <c r="AD1" s="64" t="s">
         <v>19</v>
       </c>
@@ -18600,7 +18597,7 @@
   <dimension ref="A1:AH724"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18627,37 +18624,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="1" customFormat="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="69" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="68" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="68"/>
-      <c r="J1" s="69" t="s">
+      <c r="I1" s="70"/>
+      <c r="J1" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="69" t="s">
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="66" t="s">
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="67"/>
+      <c r="S1" s="69"/>
       <c r="AD1" s="23" t="s">
         <v>19</v>
       </c>
@@ -18756,22 +18753,22 @@
         <v>25</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="N3" t="s">
+        <v>555</v>
+      </c>
+      <c r="O3" t="s">
+        <v>281</v>
+      </c>
+      <c r="P3" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q3" t="s">
         <v>280</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>283</v>
-      </c>
-      <c r="P3" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>282</v>
-      </c>
-      <c r="R3" t="s">
-        <v>285</v>
       </c>
       <c r="S3" s="31" t="s">
         <v>60</v>
@@ -18780,10 +18777,10 @@
     <row r="4" spans="1:34">
       <c r="I4" s="8"/>
       <c r="N4" t="s">
-        <v>279</v>
+        <v>556</v>
       </c>
       <c r="O4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="P4" t="s">
         <v>46</v>
@@ -18792,7 +18789,7 @@
         <v>269</v>
       </c>
       <c r="R4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="S4" s="31" t="s">
         <v>60</v>
@@ -18910,31 +18907,31 @@
     <row r="10" spans="1:34">
       <c r="I10" s="8"/>
       <c r="N10" s="21" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="Q10" s="21" t="s">
         <v>271</v>
       </c>
       <c r="R10" s="21" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="S10" s="46" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:34">
       <c r="I11" s="8"/>
       <c r="N11" s="21" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="P11" s="21" t="s">
         <v>270</v>
@@ -18943,196 +18940,196 @@
         <v>42</v>
       </c>
       <c r="R11" s="21" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="S11" s="46" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="12" spans="1:34">
       <c r="I12" s="8"/>
       <c r="N12" s="21" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="O12" s="21" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="P12" s="21" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="Q12" s="21" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="R12" s="21" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="S12" s="46" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="13" spans="1:34">
       <c r="I13" s="8"/>
       <c r="N13" s="21" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="O13" s="21" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="P13" s="21" t="s">
         <v>268</v>
       </c>
       <c r="Q13" s="21" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="R13" s="21" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="S13" s="46" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:34">
       <c r="I14" s="8"/>
       <c r="N14" s="21" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="O14" s="21" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="P14" s="21" t="s">
         <v>270</v>
       </c>
       <c r="Q14" s="21" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="R14" s="21" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="S14" s="46" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:34">
       <c r="I15" s="8"/>
       <c r="N15" s="21" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="O15" s="21" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Q15" s="21" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="R15" s="21" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="S15" s="46" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:34">
       <c r="I16" s="8"/>
       <c r="N16" s="21" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="O16" s="21" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="P16" s="21" t="s">
         <v>270</v>
       </c>
       <c r="Q16" s="21" t="s">
+        <v>518</v>
+      </c>
+      <c r="R16" s="21" t="s">
         <v>520</v>
       </c>
-      <c r="R16" s="21" t="s">
-        <v>522</v>
-      </c>
       <c r="S16" s="46" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17" spans="9:19">
       <c r="I17" s="8"/>
       <c r="N17" s="21" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="O17" s="21" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="P17" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="Q17" s="21" t="s">
         <v>271</v>
       </c>
       <c r="R17" s="21" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="S17" s="46" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="18" spans="9:19">
       <c r="I18" s="8"/>
       <c r="N18" s="21" t="s">
+        <v>522</v>
+      </c>
+      <c r="O18" s="21" t="s">
         <v>524</v>
       </c>
-      <c r="O18" s="21" t="s">
-        <v>526</v>
-      </c>
       <c r="P18" s="21" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="Q18" s="21" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="R18" s="21" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="S18" s="46" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="19" spans="9:19">
       <c r="I19" s="8"/>
       <c r="N19" s="21" t="s">
+        <v>525</v>
+      </c>
+      <c r="O19" s="21" t="s">
         <v>527</v>
-      </c>
-      <c r="O19" s="21" t="s">
-        <v>529</v>
       </c>
       <c r="P19" s="21" t="s">
         <v>268</v>
       </c>
       <c r="Q19" s="21" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="R19" s="21" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="S19" s="46" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="20" spans="9:19">
       <c r="I20" s="8"/>
       <c r="N20" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="P20" s="21" t="s">
         <v>42</v>
       </c>
       <c r="Q20" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="R20" s="78" t="s">
-        <v>545</v>
+        <v>294</v>
+      </c>
+      <c r="R20" s="66" t="s">
+        <v>543</v>
       </c>
       <c r="S20" s="31" t="s">
         <v>232</v>
@@ -19141,19 +19138,19 @@
     <row r="21" spans="9:19">
       <c r="I21" s="8"/>
       <c r="N21" t="s">
+        <v>544</v>
+      </c>
+      <c r="O21" s="21" t="s">
         <v>546</v>
       </c>
-      <c r="O21" s="21" t="s">
+      <c r="P21" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q21" s="21" t="s">
         <v>548</v>
       </c>
-      <c r="P21" s="21" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q21" s="21" t="s">
-        <v>550</v>
-      </c>
-      <c r="R21" s="78" t="s">
-        <v>551</v>
+      <c r="R21" s="66" t="s">
+        <v>549</v>
       </c>
       <c r="S21" s="31" t="s">
         <v>232</v>
@@ -19162,19 +19159,19 @@
     <row r="22" spans="9:19">
       <c r="I22" s="8"/>
       <c r="N22" t="s">
+        <v>545</v>
+      </c>
+      <c r="O22" s="21" t="s">
         <v>547</v>
       </c>
-      <c r="O22" s="21" t="s">
-        <v>549</v>
-      </c>
       <c r="P22" s="21" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="Q22" s="21" t="s">
-        <v>400</v>
-      </c>
-      <c r="R22" s="78" t="s">
-        <v>552</v>
+        <v>398</v>
+      </c>
+      <c r="R22" s="66" t="s">
+        <v>550</v>
       </c>
       <c r="S22" s="31" t="s">
         <v>232</v>
@@ -19183,7 +19180,7 @@
     <row r="23" spans="9:19">
       <c r="I23" s="8"/>
       <c r="J23" s="28" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="K23" s="28">
         <v>1472307</v>
@@ -19195,7 +19192,7 @@
         <v>42</v>
       </c>
       <c r="R23" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="S23" s="31" t="s">
         <v>232</v>
@@ -19204,7 +19201,7 @@
     <row r="24" spans="9:19">
       <c r="I24" s="8"/>
       <c r="J24" s="28" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="K24" s="28">
         <v>1472358</v>
@@ -19216,7 +19213,7 @@
         <v>42</v>
       </c>
       <c r="R24" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="S24" s="31" t="s">
         <v>232</v>
@@ -19225,7 +19222,7 @@
     <row r="25" spans="9:19">
       <c r="I25" s="8"/>
       <c r="J25" s="28" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="K25" s="28">
         <v>1472359</v>
@@ -19237,7 +19234,7 @@
         <v>45</v>
       </c>
       <c r="R25" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="S25" s="31" t="s">
         <v>232</v>
@@ -19246,7 +19243,7 @@
     <row r="26" spans="9:19">
       <c r="I26" s="8"/>
       <c r="J26" s="28" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K26" s="28">
         <v>1472359</v>
@@ -19258,7 +19255,7 @@
         <v>42</v>
       </c>
       <c r="R26" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="S26" s="31" t="s">
         <v>232</v>
@@ -19267,7 +19264,7 @@
     <row r="27" spans="9:19">
       <c r="I27" s="8"/>
       <c r="J27" s="28" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="K27" s="28">
         <v>1472362</v>
@@ -19279,7 +19276,7 @@
         <v>42</v>
       </c>
       <c r="R27" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="S27" s="31" t="s">
         <v>232</v>
@@ -19288,7 +19285,7 @@
     <row r="28" spans="9:19">
       <c r="I28" s="8"/>
       <c r="J28" s="28" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="K28" s="28">
         <v>1473246</v>
@@ -19309,7 +19306,7 @@
     <row r="29" spans="9:19">
       <c r="I29" s="8"/>
       <c r="J29" s="28" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="K29" s="28">
         <v>1473247</v>
@@ -19330,7 +19327,7 @@
     <row r="30" spans="9:19">
       <c r="I30" s="8"/>
       <c r="J30" s="28" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="K30" s="28">
         <v>1473329</v>
@@ -19351,7 +19348,7 @@
     <row r="31" spans="9:19">
       <c r="I31" s="8"/>
       <c r="J31" s="35" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="K31" s="28">
         <v>1673425</v>
@@ -19372,19 +19369,19 @@
     <row r="32" spans="9:19">
       <c r="I32" s="8"/>
       <c r="N32" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O32" s="21" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="P32" s="21" t="s">
         <v>34</v>
       </c>
       <c r="Q32" s="21" t="s">
-        <v>282</v>
-      </c>
-      <c r="R32" s="78" t="s">
-        <v>555</v>
+        <v>280</v>
+      </c>
+      <c r="R32" s="66" t="s">
+        <v>553</v>
       </c>
       <c r="S32" s="31" t="s">
         <v>128</v>
@@ -19393,19 +19390,19 @@
     <row r="33" spans="9:19">
       <c r="I33" s="8"/>
       <c r="N33" s="21" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="O33" s="21" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="P33" s="21" t="s">
         <v>270</v>
       </c>
       <c r="Q33" s="21" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="R33" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="S33" s="31" t="s">
         <v>43</v>
@@ -19414,9 +19411,9 @@
     <row r="34" spans="9:19">
       <c r="I34" s="8"/>
       <c r="J34" s="46" t="s">
-        <v>369</v>
-      </c>
-      <c r="K34" s="79">
+        <v>367</v>
+      </c>
+      <c r="K34" s="67">
         <v>2289248</v>
       </c>
       <c r="L34" s="46" t="s">
@@ -19428,8 +19425,8 @@
       <c r="O34" s="21"/>
       <c r="P34" s="21"/>
       <c r="Q34" s="21"/>
-      <c r="R34" s="78" t="s">
-        <v>371</v>
+      <c r="R34" s="66" t="s">
+        <v>369</v>
       </c>
       <c r="S34" s="46" t="s">
         <v>36</v>
@@ -19438,9 +19435,9 @@
     <row r="35" spans="9:19">
       <c r="I35" s="8"/>
       <c r="J35" s="46" t="s">
-        <v>291</v>
-      </c>
-      <c r="K35" s="79">
+        <v>289</v>
+      </c>
+      <c r="K35" s="67">
         <v>2289252</v>
       </c>
       <c r="L35" s="46" t="s">
@@ -19452,8 +19449,8 @@
       <c r="O35" s="21"/>
       <c r="P35" s="21"/>
       <c r="Q35" s="21"/>
-      <c r="R35" s="78" t="s">
-        <v>292</v>
+      <c r="R35" s="66" t="s">
+        <v>290</v>
       </c>
       <c r="S35" s="46" t="s">
         <v>36</v>
@@ -19462,9 +19459,9 @@
     <row r="36" spans="9:19">
       <c r="I36" s="8"/>
       <c r="J36" s="46" t="s">
-        <v>370</v>
-      </c>
-      <c r="K36" s="79">
+        <v>368</v>
+      </c>
+      <c r="K36" s="67">
         <v>2289253</v>
       </c>
       <c r="L36" s="46" t="s">
@@ -19476,8 +19473,8 @@
       <c r="O36" s="21"/>
       <c r="P36" s="21"/>
       <c r="Q36" s="21"/>
-      <c r="R36" s="78" t="s">
-        <v>372</v>
+      <c r="R36" s="66" t="s">
+        <v>370</v>
       </c>
       <c r="S36" s="46" t="s">
         <v>36</v>
@@ -19490,19 +19487,19 @@
       <c r="L37" s="38"/>
       <c r="M37" s="38"/>
       <c r="N37" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="O37" s="21" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="P37" s="21" t="s">
         <v>46</v>
       </c>
       <c r="Q37" s="21" t="s">
-        <v>281</v>
-      </c>
-      <c r="R37" s="78" t="s">
-        <v>294</v>
+        <v>279</v>
+      </c>
+      <c r="R37" s="66" t="s">
+        <v>292</v>
       </c>
       <c r="S37" s="46" t="s">
         <v>36</v>
@@ -19515,19 +19512,19 @@
       <c r="L38" s="38"/>
       <c r="M38" s="38"/>
       <c r="N38" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="O38" s="21" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="P38" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="Q38" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="R38" s="78" t="s">
-        <v>375</v>
+      <c r="R38" s="66" t="s">
+        <v>373</v>
       </c>
       <c r="S38" s="46" t="s">
         <v>36</v>
@@ -19540,19 +19537,19 @@
       <c r="L39" s="38"/>
       <c r="M39" s="38"/>
       <c r="N39" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O39" s="21" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="P39" s="21" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="Q39" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="R39" s="78" t="s">
-        <v>297</v>
+      <c r="R39" s="66" t="s">
+        <v>295</v>
       </c>
       <c r="S39" s="46" t="s">
         <v>36</v>
@@ -19565,10 +19562,10 @@
       <c r="L40" s="38"/>
       <c r="M40" s="38"/>
       <c r="N40" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="O40" s="21" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="P40" s="21" t="s">
         <v>269</v>
@@ -19576,8 +19573,8 @@
       <c r="Q40" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="R40" s="78" t="s">
-        <v>299</v>
+      <c r="R40" s="66" t="s">
+        <v>297</v>
       </c>
       <c r="S40" s="46" t="s">
         <v>36</v>
@@ -19590,19 +19587,19 @@
       <c r="L41" s="38"/>
       <c r="M41" s="38"/>
       <c r="N41" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="O41" s="21" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="P41" s="21" t="s">
         <v>268</v>
       </c>
       <c r="Q41" s="21" t="s">
-        <v>382</v>
-      </c>
-      <c r="R41" s="78" t="s">
-        <v>383</v>
+        <v>380</v>
+      </c>
+      <c r="R41" s="66" t="s">
+        <v>381</v>
       </c>
       <c r="S41" s="46" t="s">
         <v>36</v>
@@ -19615,19 +19612,19 @@
       <c r="L42" s="38"/>
       <c r="M42" s="38"/>
       <c r="N42" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="O42" s="21" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="Q42" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R42" s="78" t="s">
-        <v>303</v>
+      <c r="R42" s="66" t="s">
+        <v>301</v>
       </c>
       <c r="S42" s="46" t="s">
         <v>36</v>
@@ -19640,19 +19637,19 @@
       <c r="L43" s="38"/>
       <c r="M43" s="38"/>
       <c r="N43" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="O43" s="21" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="P43" s="21" t="s">
         <v>268</v>
       </c>
       <c r="Q43" s="21" t="s">
-        <v>305</v>
-      </c>
-      <c r="R43" s="78" t="s">
-        <v>384</v>
+        <v>303</v>
+      </c>
+      <c r="R43" s="66" t="s">
+        <v>382</v>
       </c>
       <c r="S43" s="46" t="s">
         <v>36</v>
@@ -19665,19 +19662,19 @@
       <c r="L44" s="38"/>
       <c r="M44" s="38"/>
       <c r="N44" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="O44" s="21" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="P44" s="21" t="s">
         <v>45</v>
       </c>
       <c r="Q44" s="21" t="s">
-        <v>307</v>
-      </c>
-      <c r="R44" s="78" t="s">
-        <v>308</v>
+        <v>305</v>
+      </c>
+      <c r="R44" s="66" t="s">
+        <v>306</v>
       </c>
       <c r="S44" s="46" t="s">
         <v>36</v>
@@ -19690,10 +19687,10 @@
       <c r="L45" s="38"/>
       <c r="M45" s="38"/>
       <c r="N45" t="s">
+        <v>383</v>
+      </c>
+      <c r="O45" s="21" t="s">
         <v>385</v>
-      </c>
-      <c r="O45" s="21" t="s">
-        <v>387</v>
       </c>
       <c r="P45" s="21" t="s">
         <v>41</v>
@@ -19701,8 +19698,8 @@
       <c r="Q45" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="R45" s="78" t="s">
-        <v>386</v>
+      <c r="R45" s="66" t="s">
+        <v>384</v>
       </c>
       <c r="S45" s="46" t="s">
         <v>36</v>
@@ -19715,19 +19712,19 @@
       <c r="L46" s="38"/>
       <c r="M46" s="38"/>
       <c r="N46" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="O46" s="21" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="P46" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="Q46" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R46" s="78" t="s">
-        <v>388</v>
+      <c r="R46" s="66" t="s">
+        <v>386</v>
       </c>
       <c r="S46" s="46" t="s">
         <v>36</v>
@@ -19740,10 +19737,10 @@
       <c r="L47" s="38"/>
       <c r="M47" s="38"/>
       <c r="N47" t="s">
+        <v>389</v>
+      </c>
+      <c r="O47" s="21" t="s">
         <v>391</v>
-      </c>
-      <c r="O47" s="21" t="s">
-        <v>393</v>
       </c>
       <c r="P47" s="21" t="s">
         <v>41</v>
@@ -19751,8 +19748,8 @@
       <c r="Q47" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="R47" s="78" t="s">
-        <v>392</v>
+      <c r="R47" s="66" t="s">
+        <v>390</v>
       </c>
       <c r="S47" s="46" t="s">
         <v>36</v>
@@ -19765,10 +19762,10 @@
       <c r="L48" s="38"/>
       <c r="M48" s="38"/>
       <c r="N48" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="O48" s="21" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="P48" s="21" t="s">
         <v>131</v>
@@ -19776,8 +19773,8 @@
       <c r="Q48" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="R48" s="78" t="s">
-        <v>310</v>
+      <c r="R48" s="66" t="s">
+        <v>308</v>
       </c>
       <c r="S48" s="46" t="s">
         <v>36</v>
@@ -19790,10 +19787,10 @@
       <c r="L49" s="38"/>
       <c r="M49" s="38"/>
       <c r="N49" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="O49" s="21" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="P49" s="21" t="s">
         <v>46</v>
@@ -19801,8 +19798,8 @@
       <c r="Q49" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="R49" s="78" t="s">
-        <v>312</v>
+      <c r="R49" s="66" t="s">
+        <v>310</v>
       </c>
       <c r="S49" s="46" t="s">
         <v>36</v>
@@ -19815,19 +19812,19 @@
       <c r="L50" s="38"/>
       <c r="M50" s="38"/>
       <c r="N50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="O50" s="21" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="P50" s="21" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="Q50" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="R50" s="78" t="s">
-        <v>314</v>
+      <c r="R50" s="66" t="s">
+        <v>312</v>
       </c>
       <c r="S50" s="46" t="s">
         <v>36</v>
@@ -19840,19 +19837,19 @@
       <c r="L51" s="38"/>
       <c r="M51" s="38"/>
       <c r="N51" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O51" s="21" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="P51" s="21" t="s">
         <v>268</v>
       </c>
       <c r="Q51" s="21" t="s">
-        <v>398</v>
-      </c>
-      <c r="R51" s="78" t="s">
-        <v>399</v>
+        <v>396</v>
+      </c>
+      <c r="R51" s="66" t="s">
+        <v>397</v>
       </c>
       <c r="S51" s="46" t="s">
         <v>36</v>
@@ -19865,19 +19862,19 @@
       <c r="L52" s="38"/>
       <c r="M52" s="38"/>
       <c r="N52" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O52" s="21" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Q52" s="21" t="s">
-        <v>400</v>
-      </c>
-      <c r="R52" s="78" t="s">
-        <v>401</v>
+        <v>398</v>
+      </c>
+      <c r="R52" s="66" t="s">
+        <v>399</v>
       </c>
       <c r="S52" s="46" t="s">
         <v>36</v>
@@ -19890,19 +19887,19 @@
       <c r="L53" s="38"/>
       <c r="M53" s="38"/>
       <c r="N53" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="O53" s="21" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="P53" s="21" t="s">
         <v>271</v>
       </c>
       <c r="Q53" s="21" t="s">
-        <v>339</v>
-      </c>
-      <c r="R53" s="78" t="s">
-        <v>405</v>
+        <v>337</v>
+      </c>
+      <c r="R53" s="66" t="s">
+        <v>403</v>
       </c>
       <c r="S53" s="46" t="s">
         <v>36</v>
@@ -19915,19 +19912,19 @@
       <c r="L54" s="38"/>
       <c r="M54" s="38"/>
       <c r="N54" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="O54" s="21" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="P54" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Q54" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="R54" s="66" t="s">
         <v>404</v>
-      </c>
-      <c r="R54" s="78" t="s">
-        <v>406</v>
       </c>
       <c r="S54" s="46" t="s">
         <v>36</v>
@@ -19940,10 +19937,10 @@
       <c r="L55" s="38"/>
       <c r="M55" s="38"/>
       <c r="N55" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="O55" s="21" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="P55" s="21" t="s">
         <v>270</v>
@@ -19951,8 +19948,8 @@
       <c r="Q55" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R55" s="78" t="s">
-        <v>410</v>
+      <c r="R55" s="66" t="s">
+        <v>408</v>
       </c>
       <c r="S55" s="46" t="s">
         <v>36</v>
@@ -19965,19 +19962,19 @@
       <c r="L56" s="38"/>
       <c r="M56" s="38"/>
       <c r="N56" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="O56" s="21" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="P56" s="21" t="s">
         <v>271</v>
       </c>
       <c r="Q56" s="21" t="s">
-        <v>411</v>
-      </c>
-      <c r="R56" s="78" t="s">
-        <v>412</v>
+        <v>409</v>
+      </c>
+      <c r="R56" s="66" t="s">
+        <v>410</v>
       </c>
       <c r="S56" s="46" t="s">
         <v>36</v>
@@ -19990,10 +19987,10 @@
       <c r="L57" s="38"/>
       <c r="M57" s="38"/>
       <c r="N57" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="O57" s="21" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="P57" s="21" t="s">
         <v>268</v>
@@ -20001,8 +19998,8 @@
       <c r="Q57" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="R57" s="78" t="s">
-        <v>322</v>
+      <c r="R57" s="66" t="s">
+        <v>320</v>
       </c>
       <c r="S57" s="46" t="s">
         <v>36</v>
@@ -20015,10 +20012,10 @@
       <c r="L58" s="38"/>
       <c r="M58" s="38"/>
       <c r="N58" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="O58" s="21" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="P58" s="21" t="s">
         <v>270</v>
@@ -20026,8 +20023,8 @@
       <c r="Q58" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R58" s="78" t="s">
-        <v>416</v>
+      <c r="R58" s="66" t="s">
+        <v>414</v>
       </c>
       <c r="S58" s="46" t="s">
         <v>36</v>
@@ -20040,10 +20037,10 @@
       <c r="L59" s="38"/>
       <c r="M59" s="38"/>
       <c r="N59" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="O59" s="21" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P59" s="21" t="s">
         <v>270</v>
@@ -20051,8 +20048,8 @@
       <c r="Q59" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R59" s="78" t="s">
-        <v>324</v>
+      <c r="R59" s="66" t="s">
+        <v>322</v>
       </c>
       <c r="S59" s="46" t="s">
         <v>36</v>
@@ -20065,19 +20062,19 @@
       <c r="L60" s="38"/>
       <c r="M60" s="38"/>
       <c r="N60" t="s">
+        <v>323</v>
+      </c>
+      <c r="O60" s="21" t="s">
+        <v>419</v>
+      </c>
+      <c r="P60" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q60" s="21" t="s">
+        <v>418</v>
+      </c>
+      <c r="R60" s="66" t="s">
         <v>325</v>
-      </c>
-      <c r="O60" s="21" t="s">
-        <v>421</v>
-      </c>
-      <c r="P60" s="21" t="s">
-        <v>326</v>
-      </c>
-      <c r="Q60" s="21" t="s">
-        <v>420</v>
-      </c>
-      <c r="R60" s="78" t="s">
-        <v>327</v>
       </c>
       <c r="S60" s="46" t="s">
         <v>36</v>
@@ -20090,19 +20087,19 @@
       <c r="L61" s="38"/>
       <c r="M61" s="38"/>
       <c r="N61" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="O61" s="21" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="P61" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Q61" s="21" t="s">
-        <v>422</v>
-      </c>
-      <c r="R61" s="78" t="s">
-        <v>423</v>
+        <v>420</v>
+      </c>
+      <c r="R61" s="66" t="s">
+        <v>421</v>
       </c>
       <c r="S61" s="46" t="s">
         <v>36</v>
@@ -20116,19 +20113,19 @@
       <c r="L62" s="38"/>
       <c r="M62" s="38"/>
       <c r="N62" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="O62" s="21" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="P62" s="21" t="s">
         <v>45</v>
       </c>
       <c r="Q62" s="21" t="s">
-        <v>307</v>
-      </c>
-      <c r="R62" s="78" t="s">
-        <v>330</v>
+        <v>305</v>
+      </c>
+      <c r="R62" s="66" t="s">
+        <v>328</v>
       </c>
       <c r="S62" s="46" t="s">
         <v>36</v>
@@ -20142,10 +20139,10 @@
       <c r="L63" s="38"/>
       <c r="M63" s="38"/>
       <c r="N63" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="O63" s="21" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="P63" s="21" t="s">
         <v>42</v>
@@ -20153,8 +20150,8 @@
       <c r="Q63" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R63" s="78" t="s">
-        <v>332</v>
+      <c r="R63" s="66" t="s">
+        <v>330</v>
       </c>
       <c r="S63" s="46" t="s">
         <v>36</v>
@@ -20167,19 +20164,19 @@
       <c r="L64" s="38"/>
       <c r="M64" s="38"/>
       <c r="N64" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O64" s="21" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="P64" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Q64" s="21" t="s">
-        <v>307</v>
-      </c>
-      <c r="R64" s="78" t="s">
-        <v>334</v>
+        <v>305</v>
+      </c>
+      <c r="R64" s="66" t="s">
+        <v>332</v>
       </c>
       <c r="S64" s="46" t="s">
         <v>36</v>
@@ -20192,19 +20189,19 @@
       <c r="L65" s="38"/>
       <c r="M65" s="38"/>
       <c r="N65" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="O65" s="21" t="s">
+        <v>426</v>
+      </c>
+      <c r="P65" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q65" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="R65" s="66" t="s">
         <v>428</v>
-      </c>
-      <c r="P65" s="21" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q65" s="21" t="s">
-        <v>336</v>
-      </c>
-      <c r="R65" s="78" t="s">
-        <v>430</v>
       </c>
       <c r="S65" s="46" t="s">
         <v>36</v>
@@ -20218,19 +20215,19 @@
       <c r="L66" s="38"/>
       <c r="M66" s="38"/>
       <c r="N66" t="s">
+        <v>335</v>
+      </c>
+      <c r="O66" s="21" t="s">
+        <v>427</v>
+      </c>
+      <c r="P66" s="21" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q66" s="21" t="s">
         <v>337</v>
       </c>
-      <c r="O66" s="21" t="s">
+      <c r="R66" s="66" t="s">
         <v>429</v>
-      </c>
-      <c r="P66" s="21" t="s">
-        <v>338</v>
-      </c>
-      <c r="Q66" s="21" t="s">
-        <v>339</v>
-      </c>
-      <c r="R66" s="78" t="s">
-        <v>431</v>
       </c>
       <c r="S66" s="46" t="s">
         <v>36</v>
@@ -20244,19 +20241,19 @@
       <c r="L67" s="38"/>
       <c r="M67" s="38"/>
       <c r="N67" t="s">
+        <v>430</v>
+      </c>
+      <c r="O67" s="21" t="s">
+        <v>433</v>
+      </c>
+      <c r="P67" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q67" s="21" t="s">
+        <v>431</v>
+      </c>
+      <c r="R67" s="66" t="s">
         <v>432</v>
-      </c>
-      <c r="O67" s="21" t="s">
-        <v>435</v>
-      </c>
-      <c r="P67" s="21" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q67" s="21" t="s">
-        <v>433</v>
-      </c>
-      <c r="R67" s="78" t="s">
-        <v>434</v>
       </c>
       <c r="S67" s="46" t="s">
         <v>36</v>
@@ -20270,19 +20267,19 @@
       <c r="L68" s="38"/>
       <c r="M68" s="38"/>
       <c r="N68" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="O68" s="21" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="P68" s="21" t="s">
         <v>41</v>
       </c>
       <c r="Q68" s="21" t="s">
-        <v>436</v>
-      </c>
-      <c r="R68" s="78" t="s">
-        <v>467</v>
+        <v>434</v>
+      </c>
+      <c r="R68" s="66" t="s">
+        <v>465</v>
       </c>
       <c r="S68" s="46" t="s">
         <v>36</v>
@@ -20296,19 +20293,19 @@
       <c r="L69" s="38"/>
       <c r="M69" s="38"/>
       <c r="N69" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="O69" s="21" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="P69" s="21" t="s">
         <v>131</v>
       </c>
       <c r="Q69" s="21" t="s">
-        <v>317</v>
-      </c>
-      <c r="R69" s="78" t="s">
-        <v>342</v>
+        <v>315</v>
+      </c>
+      <c r="R69" s="66" t="s">
+        <v>340</v>
       </c>
       <c r="S69" s="46" t="s">
         <v>36</v>
@@ -20322,19 +20319,19 @@
       <c r="L70" s="38"/>
       <c r="M70" s="38"/>
       <c r="N70" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="O70" s="21" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="P70" s="21" t="s">
         <v>270</v>
       </c>
       <c r="Q70" s="21" t="s">
-        <v>307</v>
-      </c>
-      <c r="R70" s="78" t="s">
-        <v>344</v>
+        <v>305</v>
+      </c>
+      <c r="R70" s="66" t="s">
+        <v>342</v>
       </c>
       <c r="S70" s="46" t="s">
         <v>36</v>
@@ -20347,19 +20344,19 @@
       <c r="L71" s="38"/>
       <c r="M71" s="38"/>
       <c r="N71" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="O71" s="21" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="P71" s="21" t="s">
         <v>41</v>
       </c>
       <c r="Q71" s="21" t="s">
-        <v>307</v>
-      </c>
-      <c r="R71" s="78" t="s">
-        <v>346</v>
+        <v>305</v>
+      </c>
+      <c r="R71" s="66" t="s">
+        <v>344</v>
       </c>
       <c r="S71" s="46" t="s">
         <v>36</v>
@@ -20372,19 +20369,19 @@
       <c r="L72" s="38"/>
       <c r="M72" s="38"/>
       <c r="N72" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="O72" s="21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="P72" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="Q72" s="21" t="s">
-        <v>336</v>
-      </c>
-      <c r="R72" s="78" t="s">
-        <v>440</v>
+        <v>334</v>
+      </c>
+      <c r="R72" s="66" t="s">
+        <v>438</v>
       </c>
       <c r="S72" s="46" t="s">
         <v>36</v>
@@ -20397,19 +20394,19 @@
       <c r="L73" s="38"/>
       <c r="M73" s="38"/>
       <c r="N73" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="O73" s="21" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="P73" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="Q73" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R73" s="78" t="s">
-        <v>349</v>
+      <c r="R73" s="66" t="s">
+        <v>347</v>
       </c>
       <c r="S73" s="46" t="s">
         <v>36</v>
@@ -20422,19 +20419,19 @@
       <c r="L74" s="38"/>
       <c r="M74" s="38"/>
       <c r="N74" t="s">
+        <v>441</v>
+      </c>
+      <c r="O74" s="21" t="s">
         <v>443</v>
       </c>
-      <c r="O74" s="21" t="s">
-        <v>445</v>
-      </c>
       <c r="P74" s="21" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="Q74" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R74" s="78" t="s">
-        <v>444</v>
+      <c r="R74" s="66" t="s">
+        <v>442</v>
       </c>
       <c r="S74" s="46" t="s">
         <v>36</v>
@@ -20447,19 +20444,19 @@
       <c r="L75" s="38"/>
       <c r="M75" s="38"/>
       <c r="N75" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="O75" s="21" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="P75" s="21" t="s">
         <v>269</v>
       </c>
       <c r="Q75" s="21" t="s">
-        <v>446</v>
-      </c>
-      <c r="R75" s="78" t="s">
-        <v>447</v>
+        <v>444</v>
+      </c>
+      <c r="R75" s="66" t="s">
+        <v>445</v>
       </c>
       <c r="S75" s="46" t="s">
         <v>36</v>
@@ -20472,10 +20469,10 @@
       <c r="L76" s="38"/>
       <c r="M76" s="38"/>
       <c r="N76" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="O76" s="21" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="P76" s="21" t="s">
         <v>269</v>
@@ -20483,8 +20480,8 @@
       <c r="Q76" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="R76" s="78" t="s">
-        <v>352</v>
+      <c r="R76" s="66" t="s">
+        <v>350</v>
       </c>
       <c r="S76" s="46" t="s">
         <v>36</v>
@@ -20497,19 +20494,19 @@
       <c r="L77" s="38"/>
       <c r="M77" s="38"/>
       <c r="N77" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="O77" s="21" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="P77" s="21" t="s">
         <v>41</v>
       </c>
       <c r="Q77" s="21" t="s">
-        <v>451</v>
-      </c>
-      <c r="R77" s="78" t="s">
-        <v>452</v>
+        <v>449</v>
+      </c>
+      <c r="R77" s="66" t="s">
+        <v>450</v>
       </c>
       <c r="S77" s="46" t="s">
         <v>36</v>
@@ -20522,10 +20519,10 @@
       <c r="L78" s="38"/>
       <c r="M78" s="38"/>
       <c r="N78" t="s">
+        <v>452</v>
+      </c>
+      <c r="O78" s="21" t="s">
         <v>454</v>
-      </c>
-      <c r="O78" s="21" t="s">
-        <v>456</v>
       </c>
       <c r="P78" s="21" t="s">
         <v>46</v>
@@ -20533,8 +20530,8 @@
       <c r="Q78" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="R78" s="78" t="s">
-        <v>455</v>
+      <c r="R78" s="66" t="s">
+        <v>453</v>
       </c>
       <c r="S78" s="46" t="s">
         <v>36</v>
@@ -20547,19 +20544,19 @@
       <c r="L79" s="38"/>
       <c r="M79" s="38"/>
       <c r="N79" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="O79" s="21" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="P79" s="21" t="s">
         <v>42</v>
       </c>
       <c r="Q79" s="21" t="s">
-        <v>354</v>
-      </c>
-      <c r="R79" s="78" t="s">
-        <v>465</v>
+        <v>352</v>
+      </c>
+      <c r="R79" s="66" t="s">
+        <v>463</v>
       </c>
       <c r="S79" s="46" t="s">
         <v>36</v>
@@ -20572,19 +20569,19 @@
       <c r="L80" s="38"/>
       <c r="M80" s="38"/>
       <c r="N80" t="s">
+        <v>456</v>
+      </c>
+      <c r="O80" s="21" t="s">
         <v>458</v>
       </c>
-      <c r="O80" s="21" t="s">
-        <v>460</v>
-      </c>
       <c r="P80" s="21" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="Q80" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R80" s="78" t="s">
-        <v>459</v>
+      <c r="R80" s="66" t="s">
+        <v>457</v>
       </c>
       <c r="S80" s="46" t="s">
         <v>36</v>
@@ -20597,10 +20594,10 @@
       <c r="L81" s="38"/>
       <c r="M81" s="38"/>
       <c r="N81" t="s">
+        <v>459</v>
+      </c>
+      <c r="O81" s="21" t="s">
         <v>461</v>
-      </c>
-      <c r="O81" s="21" t="s">
-        <v>463</v>
       </c>
       <c r="P81" s="21" t="s">
         <v>45</v>
@@ -20608,8 +20605,8 @@
       <c r="Q81" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="R81" s="78" t="s">
-        <v>462</v>
+      <c r="R81" s="66" t="s">
+        <v>460</v>
       </c>
       <c r="S81" s="46" t="s">
         <v>36</v>
@@ -20622,19 +20619,19 @@
       <c r="L82" s="38"/>
       <c r="M82" s="38"/>
       <c r="N82" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="O82" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="P82" s="21" t="s">
         <v>269</v>
       </c>
       <c r="Q82" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="R82" s="78" t="s">
-        <v>466</v>
+        <v>354</v>
+      </c>
+      <c r="R82" s="66" t="s">
+        <v>464</v>
       </c>
       <c r="S82" s="46" t="s">
         <v>36</v>
@@ -20647,19 +20644,19 @@
       <c r="L83" s="38"/>
       <c r="M83" s="38"/>
       <c r="N83" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O83" s="21" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="P83" s="21" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="Q83" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R83" s="78" t="s">
-        <v>358</v>
+      <c r="R83" s="66" t="s">
+        <v>356</v>
       </c>
       <c r="S83" s="46" t="s">
         <v>36</v>
@@ -20672,19 +20669,19 @@
       <c r="L84" s="38"/>
       <c r="M84" s="38"/>
       <c r="N84" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="O84" s="21" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="P84" s="21" t="s">
         <v>42</v>
       </c>
       <c r="Q84" s="21" t="s">
-        <v>360</v>
-      </c>
-      <c r="R84" s="78" t="s">
-        <v>470</v>
+        <v>358</v>
+      </c>
+      <c r="R84" s="66" t="s">
+        <v>468</v>
       </c>
       <c r="S84" s="46" t="s">
         <v>36</v>
@@ -20697,19 +20694,19 @@
       <c r="L85" s="38"/>
       <c r="M85" s="38"/>
       <c r="N85" t="s">
+        <v>469</v>
+      </c>
+      <c r="O85" s="21" t="s">
         <v>471</v>
       </c>
-      <c r="O85" s="21" t="s">
-        <v>473</v>
-      </c>
       <c r="P85" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="Q85" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="R85" s="78" t="s">
-        <v>472</v>
+      <c r="R85" s="66" t="s">
+        <v>470</v>
       </c>
       <c r="S85" s="46" t="s">
         <v>36</v>
@@ -20723,10 +20720,10 @@
       <c r="L86" s="38"/>
       <c r="M86" s="38"/>
       <c r="N86" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="O86" s="21" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="P86" s="21" t="s">
         <v>269</v>
@@ -20734,8 +20731,8 @@
       <c r="Q86" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="R86" s="78" t="s">
-        <v>362</v>
+      <c r="R86" s="66" t="s">
+        <v>360</v>
       </c>
       <c r="S86" s="46" t="s">
         <v>36</v>
@@ -20750,19 +20747,19 @@
       <c r="L87" s="38"/>
       <c r="M87" s="38"/>
       <c r="N87" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="O87" s="21" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="P87" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="Q87" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R87" s="78" t="s">
-        <v>479</v>
+      <c r="R87" s="66" t="s">
+        <v>477</v>
       </c>
       <c r="S87" s="46" t="s">
         <v>36</v>
@@ -20777,10 +20774,10 @@
       <c r="L88" s="38"/>
       <c r="M88" s="38"/>
       <c r="N88" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="O88" s="21" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="P88" s="21" t="s">
         <v>42</v>
@@ -20788,8 +20785,8 @@
       <c r="Q88" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R88" s="78" t="s">
-        <v>482</v>
+      <c r="R88" s="66" t="s">
+        <v>480</v>
       </c>
       <c r="S88" s="46" t="s">
         <v>36</v>
@@ -20804,10 +20801,10 @@
       <c r="L89" s="38"/>
       <c r="M89" s="38"/>
       <c r="N89" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="O89" s="21" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="P89" s="21" t="s">
         <v>41</v>
@@ -20815,8 +20812,8 @@
       <c r="Q89" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="R89" s="78" t="s">
-        <v>484</v>
+      <c r="R89" s="66" t="s">
+        <v>482</v>
       </c>
       <c r="S89" s="46" t="s">
         <v>36</v>
@@ -20831,10 +20828,10 @@
       <c r="L90" s="38"/>
       <c r="M90" s="38"/>
       <c r="N90" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="O90" s="21" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="P90" s="21" t="s">
         <v>42</v>
@@ -20842,8 +20839,8 @@
       <c r="Q90" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R90" s="78" t="s">
-        <v>486</v>
+      <c r="R90" s="66" t="s">
+        <v>484</v>
       </c>
       <c r="S90" s="46" t="s">
         <v>36</v>
@@ -20858,19 +20855,19 @@
       <c r="L91" s="38"/>
       <c r="M91" s="38"/>
       <c r="N91" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="O91" s="21" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="P91" s="21" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="Q91" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="R91" s="78" t="s">
-        <v>364</v>
+      <c r="R91" s="66" t="s">
+        <v>362</v>
       </c>
       <c r="S91" s="46" t="s">
         <v>36</v>
@@ -20883,19 +20880,19 @@
       <c r="L92" s="38"/>
       <c r="M92" s="38"/>
       <c r="N92" t="s">
+        <v>363</v>
+      </c>
+      <c r="O92" s="21" t="s">
+        <v>487</v>
+      </c>
+      <c r="P92" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q92" s="21" t="s">
+        <v>486</v>
+      </c>
+      <c r="R92" s="66" t="s">
         <v>365</v>
-      </c>
-      <c r="O92" s="21" t="s">
-        <v>489</v>
-      </c>
-      <c r="P92" s="21" t="s">
-        <v>366</v>
-      </c>
-      <c r="Q92" s="21" t="s">
-        <v>488</v>
-      </c>
-      <c r="R92" s="78" t="s">
-        <v>367</v>
       </c>
       <c r="S92" s="46" t="s">
         <v>36</v>
@@ -20909,19 +20906,19 @@
       <c r="L93" s="38"/>
       <c r="M93" s="38"/>
       <c r="N93" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="O93" s="21" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="P93" s="21" t="s">
         <v>269</v>
       </c>
       <c r="Q93" s="21" t="s">
-        <v>446</v>
-      </c>
-      <c r="R93" s="78" t="s">
-        <v>492</v>
+        <v>444</v>
+      </c>
+      <c r="R93" s="66" t="s">
+        <v>490</v>
       </c>
       <c r="S93" s="46" t="s">
         <v>36</v>
@@ -25164,12 +25161,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="R1:S1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4">

</xml_diff>

<commit_message>
In TB WHO output change rpoB nomenclature to TB instead of Ecoli
</commit_message>
<xml_diff>
--- a/assay_data/TB_assays.xlsx
+++ b/assay_data/TB_assays.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21960" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="9060" yWindow="3860" windowWidth="38400" windowHeight="21960" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TB" sheetId="1" r:id="rId1"/>
@@ -2412,44 +2412,270 @@
     <t>pncA V180 mutation present which is associated with pyrazinamide resistance.</t>
   </si>
   <si>
-    <t>L511</t>
-  </si>
-  <si>
-    <t>Q513</t>
-  </si>
-  <si>
     <t>K,L,P</t>
   </si>
   <si>
-    <t>D516</t>
-  </si>
-  <si>
-    <t>S522</t>
-  </si>
-  <si>
     <t>Q,L</t>
   </si>
   <si>
-    <t>H526</t>
-  </si>
-  <si>
-    <t>S531</t>
-  </si>
-  <si>
-    <t>L533</t>
-  </si>
-  <si>
     <t>Rifampicin</t>
   </si>
   <si>
-    <t>rpoB L511P mutation present which is associated with rifampicin resistance. Minimal-confidence mutation in Miotto et al. 2017.</t>
-  </si>
-  <si>
     <t>katG S315 mutation present which is associated with isoniazid resistance.</t>
   </si>
   <si>
+    <t>761094-761096</t>
+  </si>
+  <si>
+    <t>761100-761102</t>
+  </si>
+  <si>
+    <t>761097-761099</t>
+  </si>
+  <si>
+    <t>A,F,G,N,V,Y</t>
+  </si>
+  <si>
+    <t>761109-761111</t>
+  </si>
+  <si>
+    <t>761127-761129</t>
+  </si>
+  <si>
+    <t>C,D,F,G,L,N,R,Y</t>
+  </si>
+  <si>
+    <t>761139-761141</t>
+  </si>
+  <si>
+    <t>F,L,Q,W,Y</t>
+  </si>
+  <si>
+    <t>761154-761156</t>
+  </si>
+  <si>
+    <t>761160-761162</t>
+  </si>
+  <si>
+    <t>761277-761279</t>
+  </si>
+  <si>
+    <t>761439-761441</t>
+  </si>
+  <si>
+    <t>a1401g</t>
+  </si>
+  <si>
+    <t>c1402t</t>
+  </si>
+  <si>
+    <t>g1484t</t>
+  </si>
+  <si>
+    <t>a514c</t>
+  </si>
+  <si>
+    <t>a514t</t>
+  </si>
+  <si>
+    <t>rrs a514t mutation present which is associated with streptomycin resistance.</t>
+  </si>
+  <si>
+    <t>rrs a514c mutation present which is associated with streptomycin resistance.</t>
+  </si>
+  <si>
+    <t>c513t</t>
+  </si>
+  <si>
+    <t>rrs c513t mutation present which is associated with streptomycin resistance.</t>
+  </si>
+  <si>
+    <t>c517t</t>
+  </si>
+  <si>
+    <t>rrs c517t mutation present which is associated with streptomycin resistance.</t>
+  </si>
+  <si>
+    <t>c462t</t>
+  </si>
+  <si>
+    <t>rrs c462t mutation present which is associated with streptomycin resistance.</t>
+  </si>
+  <si>
+    <t>T40</t>
+  </si>
+  <si>
+    <t>781677-781679</t>
+  </si>
+  <si>
+    <t>rpsL T40I mutation present which is associated with streptomycin resistance.</t>
+  </si>
+  <si>
+    <t>K43</t>
+  </si>
+  <si>
+    <t>K88</t>
+  </si>
+  <si>
+    <t>781686-781688</t>
+  </si>
+  <si>
+    <t>781821-781823</t>
+  </si>
+  <si>
+    <t>R,T</t>
+  </si>
+  <si>
+    <t>rpsL K43 mutation present which is associated with streptomycin resistance.</t>
+  </si>
+  <si>
+    <t>rpsL K88 mutation present which is associated with streptomycin resistance.</t>
+  </si>
+  <si>
+    <t>N236</t>
+  </si>
+  <si>
+    <t>1918645-1918647</t>
+  </si>
+  <si>
+    <t>tlyA N236K mutation present which is associated with capreomycin resistance.</t>
+  </si>
+  <si>
+    <t>references/ASM19595v2.fasta</t>
+  </si>
+  <si>
+    <t>E459</t>
+  </si>
+  <si>
+    <t>A504</t>
+  </si>
+  <si>
+    <t>L430</t>
+  </si>
+  <si>
+    <t>S431</t>
+  </si>
+  <si>
+    <t>Q432</t>
+  </si>
+  <si>
+    <t>D435</t>
+  </si>
+  <si>
+    <t>H445</t>
+  </si>
+  <si>
+    <t>S441</t>
+  </si>
+  <si>
+    <t>S450</t>
+  </si>
+  <si>
+    <t>L452</t>
+  </si>
+  <si>
+    <t>I491</t>
+  </si>
+  <si>
+    <t>rpoB L430P (L511P) mutation present which is associated with rifampicin resistance. Minimal-confidence mutation in Miotto et al. 2017.</t>
+  </si>
+  <si>
+    <t>rpoB S431T (S512T) mutation present which is associated with rifampicin resistance.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">rpoB L533P mutation present which is associated with rifampicin resistance. Moderate-confidence mutation in Miotto </t>
+      <t xml:space="preserve">rpoB Q432 (Q513) mutation present which is associated with rifampicin resistance. Q513K, Q513L, and Q513P are high-confidence mutations in Miotto </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. 2017.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rpoB D435 (D516) mutation present which is associated with rifampicin resistance. D516A, D516F, D516G andD516V are high-confidence mutations in Miotto </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>et al.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2017. D516Y is a moderate-confidence mutation in Miotto et al. 2017</t>
+    </r>
+  </si>
+  <si>
+    <t>rpoB S441 (S522) mutation present which is associated with rifampicin resistance. S522Q is a high-confidence mutation in Miotto et al. 2017. S522L is a moderate-confidence mutation in Miotto et al. 2017.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rpoB H445 (H526) mutation present which is associated with rifampicin resistance. H526C, H526D, H526G, H526L, H526R, and H526Y mutations are high-confidence mutations in Miotto et al. 2017. H526N is a minimal-confidence mutation in Miotto </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. 2017</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rpoB S450 (S531) mutation present which is associated with rifampicin resistance. S531F, S531L, S531W are high-confidence mutations in Miotto </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>et al</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. 2017.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rpoB L452P (L533P) mutation present which is associated with rifampicin resistance. Moderate-confidence mutation in Miotto </t>
     </r>
     <r>
       <rPr>
@@ -2470,239 +2696,13 @@
     </r>
   </si>
   <si>
-    <t>761094-761096</t>
-  </si>
-  <si>
-    <t>761100-761102</t>
-  </si>
-  <si>
-    <t>S512</t>
-  </si>
-  <si>
-    <t>761097-761099</t>
-  </si>
-  <si>
-    <t>rpoB S512T mutation present which is associated with rifampicin resistance.</t>
-  </si>
-  <si>
-    <t>A,F,G,N,V,Y</t>
-  </si>
-  <si>
-    <t>761109-761111</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">rpoB Q513 mutation present which is associated with rifampicin resistance. Q513K, Q513L, and Q513P are high-confidence mutations in Miotto </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>et al</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. 2017.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">rpoB D516 mutation present which is associated with rifampicin resistance. D516A, D516F, D516G andD516V are high-confidence mutations in Miotto </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>et al.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 2017. D516Y is a moderate-confidence mutation in Miotto et al. 2017</t>
-    </r>
-  </si>
-  <si>
-    <t>rpoB S522 mutation present which is associated with rifampicin resistance. S522Q is a high-confidence mutation in Miotto et al. 2017. S522L is a moderate-confidence mutation in Miotto et al. 2017.</t>
-  </si>
-  <si>
-    <t>761127-761129</t>
-  </si>
-  <si>
-    <t>C,D,F,G,L,N,R,Y</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">rpoB H526 mutation present which is associated with rifampicin resistance. H526C, H526D, H526G, H526L, H526R, and H526Y mutations are high-confidence mutations in Miotto et al. 2017. H526N is a minimal-confidence mutation in Miotto </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>et al</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. 2017</t>
-    </r>
-  </si>
-  <si>
-    <t>761139-761141</t>
-  </si>
-  <si>
-    <t>F,L,Q,W,Y</t>
-  </si>
-  <si>
-    <t>761154-761156</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">rpoB S531 mutation present which is associated with rifampicin resistance. S531F, S531L, S531W are high-confidence mutations in Miotto </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>et al</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. 2017.</t>
-    </r>
-  </si>
-  <si>
-    <t>761160-761162</t>
-  </si>
-  <si>
-    <t>I572</t>
-  </si>
-  <si>
-    <t>rpoB I572F mutation present which is associated with rifampicin resistance. Minimal-confidence mutation in Miotto et al. 2017.</t>
-  </si>
-  <si>
-    <t>761277-761279</t>
-  </si>
-  <si>
-    <t>D626</t>
-  </si>
-  <si>
-    <t>rpoB D626E mutation present which is associated with rifampicin resistance.</t>
-  </si>
-  <si>
-    <t>761439-761441</t>
-  </si>
-  <si>
-    <t>a1401g</t>
-  </si>
-  <si>
-    <t>c1402t</t>
-  </si>
-  <si>
-    <t>g1484t</t>
-  </si>
-  <si>
-    <t>a514c</t>
-  </si>
-  <si>
-    <t>a514t</t>
-  </si>
-  <si>
-    <t>rrs a514t mutation present which is associated with streptomycin resistance.</t>
-  </si>
-  <si>
-    <t>rrs a514c mutation present which is associated with streptomycin resistance.</t>
-  </si>
-  <si>
-    <t>c513t</t>
-  </si>
-  <si>
-    <t>rrs c513t mutation present which is associated with streptomycin resistance.</t>
-  </si>
-  <si>
-    <t>c517t</t>
-  </si>
-  <si>
-    <t>rrs c517t mutation present which is associated with streptomycin resistance.</t>
-  </si>
-  <si>
-    <t>c462t</t>
-  </si>
-  <si>
-    <t>rrs c462t mutation present which is associated with streptomycin resistance.</t>
-  </si>
-  <si>
-    <t>T40</t>
-  </si>
-  <si>
-    <t>781677-781679</t>
-  </si>
-  <si>
-    <t>rpsL T40I mutation present which is associated with streptomycin resistance.</t>
-  </si>
-  <si>
-    <t>K43</t>
-  </si>
-  <si>
-    <t>K88</t>
-  </si>
-  <si>
-    <t>781686-781688</t>
-  </si>
-  <si>
-    <t>781821-781823</t>
-  </si>
-  <si>
-    <t>R,T</t>
-  </si>
-  <si>
-    <t>rpsL K43 mutation present which is associated with streptomycin resistance.</t>
-  </si>
-  <si>
-    <t>rpsL K88 mutation present which is associated with streptomycin resistance.</t>
-  </si>
-  <si>
-    <t>N236</t>
-  </si>
-  <si>
-    <t>1918645-1918647</t>
-  </si>
-  <si>
-    <t>tlyA N236K mutation present which is associated with capreomycin resistance.</t>
-  </si>
-  <si>
-    <t>references/ASM19595v2.fasta</t>
-  </si>
-  <si>
-    <t>E459</t>
-  </si>
-  <si>
-    <t>A504</t>
+    <t>rpoB I491F (I572F) mutation present which is associated with rifampicin resistance. Minimal-confidence mutation in Miotto et al. 2017.</t>
+  </si>
+  <si>
+    <t>D545</t>
+  </si>
+  <si>
+    <t>rpoB D545E (D626E) mutation present which is associated with rifampicin resistance.</t>
   </si>
 </sst>
 </file>
@@ -18597,7 +18597,7 @@
   <dimension ref="A1:AH724"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18753,10 +18753,10 @@
         <v>25</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>554</v>
+        <v>534</v>
       </c>
       <c r="N3" t="s">
-        <v>555</v>
+        <v>535</v>
       </c>
       <c r="O3" t="s">
         <v>281</v>
@@ -18777,7 +18777,7 @@
     <row r="4" spans="1:34">
       <c r="I4" s="8"/>
       <c r="N4" t="s">
-        <v>556</v>
+        <v>536</v>
       </c>
       <c r="O4" t="s">
         <v>282</v>
@@ -18907,10 +18907,10 @@
     <row r="10" spans="1:34">
       <c r="I10" s="8"/>
       <c r="N10" s="21" t="s">
-        <v>491</v>
+        <v>537</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="P10" s="21" t="s">
         <v>317</v>
@@ -18919,19 +18919,19 @@
         <v>271</v>
       </c>
       <c r="R10" s="21" t="s">
-        <v>501</v>
+        <v>546</v>
       </c>
       <c r="S10" s="46" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="11" spans="1:34">
       <c r="I11" s="8"/>
       <c r="N11" s="21" t="s">
-        <v>506</v>
+        <v>538</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
       <c r="P11" s="21" t="s">
         <v>270</v>
@@ -18940,124 +18940,124 @@
         <v>42</v>
       </c>
       <c r="R11" s="21" t="s">
-        <v>508</v>
+        <v>547</v>
       </c>
       <c r="S11" s="46" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="12" spans="1:34">
       <c r="I12" s="8"/>
       <c r="N12" s="21" t="s">
-        <v>492</v>
+        <v>539</v>
       </c>
       <c r="O12" s="21" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="P12" s="21" t="s">
         <v>300</v>
       </c>
       <c r="Q12" s="21" t="s">
+        <v>491</v>
+      </c>
+      <c r="R12" s="21" t="s">
+        <v>548</v>
+      </c>
+      <c r="S12" s="46" t="s">
         <v>493</v>
-      </c>
-      <c r="R12" s="21" t="s">
-        <v>511</v>
-      </c>
-      <c r="S12" s="46" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="13" spans="1:34">
       <c r="I13" s="8"/>
       <c r="N13" s="21" t="s">
-        <v>494</v>
+        <v>540</v>
       </c>
       <c r="O13" s="21" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
       <c r="P13" s="21" t="s">
         <v>268</v>
       </c>
       <c r="Q13" s="21" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
       <c r="R13" s="21" t="s">
-        <v>512</v>
+        <v>549</v>
       </c>
       <c r="S13" s="46" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="14" spans="1:34">
       <c r="I14" s="8"/>
       <c r="N14" s="21" t="s">
-        <v>495</v>
+        <v>542</v>
       </c>
       <c r="O14" s="21" t="s">
-        <v>514</v>
+        <v>500</v>
       </c>
       <c r="P14" s="21" t="s">
         <v>270</v>
       </c>
       <c r="Q14" s="21" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="R14" s="21" t="s">
-        <v>513</v>
+        <v>550</v>
       </c>
       <c r="S14" s="46" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="15" spans="1:34">
       <c r="I15" s="8"/>
       <c r="N15" s="21" t="s">
-        <v>497</v>
+        <v>541</v>
       </c>
       <c r="O15" s="21" t="s">
-        <v>517</v>
+        <v>502</v>
       </c>
       <c r="P15" s="21" t="s">
         <v>315</v>
       </c>
       <c r="Q15" s="21" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="R15" s="21" t="s">
-        <v>516</v>
+        <v>551</v>
       </c>
       <c r="S15" s="46" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="16" spans="1:34">
       <c r="I16" s="8"/>
       <c r="N16" s="21" t="s">
-        <v>498</v>
+        <v>543</v>
       </c>
       <c r="O16" s="21" t="s">
-        <v>519</v>
+        <v>504</v>
       </c>
       <c r="P16" s="21" t="s">
         <v>270</v>
       </c>
       <c r="Q16" s="21" t="s">
-        <v>518</v>
+        <v>503</v>
       </c>
       <c r="R16" s="21" t="s">
-        <v>520</v>
+        <v>552</v>
       </c>
       <c r="S16" s="46" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="17" spans="9:19">
       <c r="I17" s="8"/>
       <c r="N17" s="21" t="s">
-        <v>499</v>
+        <v>544</v>
       </c>
       <c r="O17" s="21" t="s">
-        <v>521</v>
+        <v>505</v>
       </c>
       <c r="P17" s="21" t="s">
         <v>317</v>
@@ -19066,19 +19066,19 @@
         <v>271</v>
       </c>
       <c r="R17" s="21" t="s">
-        <v>503</v>
+        <v>553</v>
       </c>
       <c r="S17" s="46" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="18" spans="9:19">
       <c r="I18" s="8"/>
       <c r="N18" s="21" t="s">
-        <v>522</v>
+        <v>545</v>
       </c>
       <c r="O18" s="21" t="s">
-        <v>524</v>
+        <v>506</v>
       </c>
       <c r="P18" s="21" t="s">
         <v>294</v>
@@ -19087,19 +19087,19 @@
         <v>336</v>
       </c>
       <c r="R18" s="21" t="s">
-        <v>523</v>
+        <v>554</v>
       </c>
       <c r="S18" s="46" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="19" spans="9:19">
       <c r="I19" s="8"/>
       <c r="N19" s="21" t="s">
-        <v>525</v>
+        <v>555</v>
       </c>
       <c r="O19" s="21" t="s">
-        <v>527</v>
+        <v>507</v>
       </c>
       <c r="P19" s="21" t="s">
         <v>268</v>
@@ -19108,19 +19108,19 @@
         <v>279</v>
       </c>
       <c r="R19" s="21" t="s">
-        <v>526</v>
+        <v>556</v>
       </c>
       <c r="S19" s="46" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="20" spans="9:19">
       <c r="I20" s="8"/>
       <c r="N20" t="s">
-        <v>541</v>
+        <v>521</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>542</v>
+        <v>522</v>
       </c>
       <c r="P20" s="21" t="s">
         <v>42</v>
@@ -19129,7 +19129,7 @@
         <v>294</v>
       </c>
       <c r="R20" s="66" t="s">
-        <v>543</v>
+        <v>523</v>
       </c>
       <c r="S20" s="31" t="s">
         <v>232</v>
@@ -19138,19 +19138,19 @@
     <row r="21" spans="9:19">
       <c r="I21" s="8"/>
       <c r="N21" t="s">
-        <v>544</v>
+        <v>524</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>546</v>
+        <v>526</v>
       </c>
       <c r="P21" s="21" t="s">
         <v>280</v>
       </c>
       <c r="Q21" s="21" t="s">
-        <v>548</v>
+        <v>528</v>
       </c>
       <c r="R21" s="66" t="s">
-        <v>549</v>
+        <v>529</v>
       </c>
       <c r="S21" s="31" t="s">
         <v>232</v>
@@ -19159,10 +19159,10 @@
     <row r="22" spans="9:19">
       <c r="I22" s="8"/>
       <c r="N22" t="s">
-        <v>545</v>
+        <v>525</v>
       </c>
       <c r="O22" s="21" t="s">
-        <v>547</v>
+        <v>527</v>
       </c>
       <c r="P22" s="21" t="s">
         <v>280</v>
@@ -19171,7 +19171,7 @@
         <v>398</v>
       </c>
       <c r="R22" s="66" t="s">
-        <v>550</v>
+        <v>530</v>
       </c>
       <c r="S22" s="31" t="s">
         <v>232</v>
@@ -19180,7 +19180,7 @@
     <row r="23" spans="9:19">
       <c r="I23" s="8"/>
       <c r="J23" s="28" t="s">
-        <v>539</v>
+        <v>519</v>
       </c>
       <c r="K23" s="28">
         <v>1472307</v>
@@ -19192,7 +19192,7 @@
         <v>42</v>
       </c>
       <c r="R23" t="s">
-        <v>540</v>
+        <v>520</v>
       </c>
       <c r="S23" s="31" t="s">
         <v>232</v>
@@ -19201,7 +19201,7 @@
     <row r="24" spans="9:19">
       <c r="I24" s="8"/>
       <c r="J24" s="28" t="s">
-        <v>535</v>
+        <v>515</v>
       </c>
       <c r="K24" s="28">
         <v>1472358</v>
@@ -19213,7 +19213,7 @@
         <v>42</v>
       </c>
       <c r="R24" t="s">
-        <v>536</v>
+        <v>516</v>
       </c>
       <c r="S24" s="31" t="s">
         <v>232</v>
@@ -19222,7 +19222,7 @@
     <row r="25" spans="9:19">
       <c r="I25" s="8"/>
       <c r="J25" s="28" t="s">
-        <v>531</v>
+        <v>511</v>
       </c>
       <c r="K25" s="28">
         <v>1472359</v>
@@ -19234,7 +19234,7 @@
         <v>45</v>
       </c>
       <c r="R25" t="s">
-        <v>534</v>
+        <v>514</v>
       </c>
       <c r="S25" s="31" t="s">
         <v>232</v>
@@ -19243,7 +19243,7 @@
     <row r="26" spans="9:19">
       <c r="I26" s="8"/>
       <c r="J26" s="28" t="s">
-        <v>532</v>
+        <v>512</v>
       </c>
       <c r="K26" s="28">
         <v>1472359</v>
@@ -19255,7 +19255,7 @@
         <v>42</v>
       </c>
       <c r="R26" t="s">
-        <v>533</v>
+        <v>513</v>
       </c>
       <c r="S26" s="31" t="s">
         <v>232</v>
@@ -19264,7 +19264,7 @@
     <row r="27" spans="9:19">
       <c r="I27" s="8"/>
       <c r="J27" s="28" t="s">
-        <v>537</v>
+        <v>517</v>
       </c>
       <c r="K27" s="28">
         <v>1472362</v>
@@ -19276,7 +19276,7 @@
         <v>42</v>
       </c>
       <c r="R27" t="s">
-        <v>538</v>
+        <v>518</v>
       </c>
       <c r="S27" s="31" t="s">
         <v>232</v>
@@ -19285,7 +19285,7 @@
     <row r="28" spans="9:19">
       <c r="I28" s="8"/>
       <c r="J28" s="28" t="s">
-        <v>528</v>
+        <v>508</v>
       </c>
       <c r="K28" s="28">
         <v>1473246</v>
@@ -19306,7 +19306,7 @@
     <row r="29" spans="9:19">
       <c r="I29" s="8"/>
       <c r="J29" s="28" t="s">
-        <v>529</v>
+        <v>509</v>
       </c>
       <c r="K29" s="28">
         <v>1473247</v>
@@ -19327,7 +19327,7 @@
     <row r="30" spans="9:19">
       <c r="I30" s="8"/>
       <c r="J30" s="28" t="s">
-        <v>530</v>
+        <v>510</v>
       </c>
       <c r="K30" s="28">
         <v>1473329</v>
@@ -19369,10 +19369,10 @@
     <row r="32" spans="9:19">
       <c r="I32" s="8"/>
       <c r="N32" t="s">
-        <v>551</v>
+        <v>531</v>
       </c>
       <c r="O32" s="21" t="s">
-        <v>552</v>
+        <v>532</v>
       </c>
       <c r="P32" s="21" t="s">
         <v>34</v>
@@ -19381,7 +19381,7 @@
         <v>280</v>
       </c>
       <c r="R32" s="66" t="s">
-        <v>553</v>
+        <v>533</v>
       </c>
       <c r="S32" s="31" t="s">
         <v>128</v>
@@ -19402,7 +19402,7 @@
         <v>288</v>
       </c>
       <c r="R33" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="S33" s="31" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
TB_WHO: change SNP names to match format: PosRef>Alt instead of RefPosAlt
</commit_message>
<xml_diff>
--- a/assay_data/TB_assays.xlsx
+++ b/assay_data/TB_assays.xlsx
@@ -1713,18 +1713,6 @@
     <t>TB_AMR</t>
   </si>
   <si>
-    <t>g-10a</t>
-  </si>
-  <si>
-    <t>c-12t</t>
-  </si>
-  <si>
-    <t>c-14t</t>
-  </si>
-  <si>
-    <t>g-37t</t>
-  </si>
-  <si>
     <t>G88</t>
   </si>
   <si>
@@ -1794,9 +1782,6 @@
     <t>gyrB 504 mutation present which is associated with resistance to quinolones, but Moxifloxacin may still have clinical activity. Testing for MOX MIC is recommended.</t>
   </si>
   <si>
-    <t>c-15t</t>
-  </si>
-  <si>
     <t>S315</t>
   </si>
   <si>
@@ -1806,9 +1791,6 @@
     <t>I,N,T</t>
   </si>
   <si>
-    <t>a-11g</t>
-  </si>
-  <si>
     <t>pncA a-11g mutation present which is associated with pyrazinamide resistance. High-confidence mutation in Miotto et al. 2017.</t>
   </si>
   <si>
@@ -2040,12 +2022,6 @@
     <t>2289235-2289233</t>
   </si>
   <si>
-    <t>t-7c</t>
-  </si>
-  <si>
-    <t>t-12c</t>
-  </si>
-  <si>
     <t>pncA t-7c mutation present which is associated with pyrazinamide resistance. High-confidence mutation in Miotto et al. 2017.</t>
   </si>
   <si>
@@ -2463,40 +2439,16 @@
     <t>761439-761441</t>
   </si>
   <si>
-    <t>a1401g</t>
-  </si>
-  <si>
-    <t>c1402t</t>
-  </si>
-  <si>
-    <t>g1484t</t>
-  </si>
-  <si>
-    <t>a514c</t>
-  </si>
-  <si>
-    <t>a514t</t>
-  </si>
-  <si>
     <t>rrs a514t mutation present which is associated with streptomycin resistance.</t>
   </si>
   <si>
     <t>rrs a514c mutation present which is associated with streptomycin resistance.</t>
   </si>
   <si>
-    <t>c513t</t>
-  </si>
-  <si>
     <t>rrs c513t mutation present which is associated with streptomycin resistance.</t>
   </si>
   <si>
-    <t>c517t</t>
-  </si>
-  <si>
     <t>rrs c517t mutation present which is associated with streptomycin resistance.</t>
-  </si>
-  <si>
-    <t>c462t</t>
   </si>
   <si>
     <t>rrs c462t mutation present which is associated with streptomycin resistance.</t>
@@ -2703,6 +2655,54 @@
   </si>
   <si>
     <t>rpoB D545E (D626E) mutation present which is associated with rifampicin resistance.</t>
+  </si>
+  <si>
+    <t>462C&gt;T</t>
+  </si>
+  <si>
+    <t>513C&gt;T</t>
+  </si>
+  <si>
+    <t>514A&gt;C</t>
+  </si>
+  <si>
+    <t>514A&gt;T</t>
+  </si>
+  <si>
+    <t>517C&gt;T</t>
+  </si>
+  <si>
+    <t>1401A&gt;G</t>
+  </si>
+  <si>
+    <t>1402C&gt;T</t>
+  </si>
+  <si>
+    <t>1484G&gt;T</t>
+  </si>
+  <si>
+    <t>-15C&gt;T</t>
+  </si>
+  <si>
+    <t>-7T&gt;C</t>
+  </si>
+  <si>
+    <t>-11A&gt;G</t>
+  </si>
+  <si>
+    <t>-12T&gt;C</t>
+  </si>
+  <si>
+    <t>-10G&gt;A</t>
+  </si>
+  <si>
+    <t>-12C&gt;T</t>
+  </si>
+  <si>
+    <t>-14C&gt;T</t>
+  </si>
+  <si>
+    <t>-37G&gt;T</t>
   </si>
 </sst>
 </file>
@@ -3412,7 +3412,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3606,6 +3606,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="449">
@@ -18597,7 +18600,7 @@
   <dimension ref="A1:AH724"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18753,22 +18756,22 @@
         <v>25</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
       <c r="N3" t="s">
-        <v>535</v>
+        <v>519</v>
       </c>
       <c r="O3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="P3" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>276</v>
+      </c>
+      <c r="R3" t="s">
         <v>279</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>280</v>
-      </c>
-      <c r="R3" t="s">
-        <v>283</v>
       </c>
       <c r="S3" s="31" t="s">
         <v>60</v>
@@ -18777,19 +18780,19 @@
     <row r="4" spans="1:34">
       <c r="I4" s="8"/>
       <c r="N4" t="s">
-        <v>536</v>
+        <v>520</v>
       </c>
       <c r="O4" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="P4" t="s">
         <v>46</v>
       </c>
       <c r="Q4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="R4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="S4" s="31" t="s">
         <v>60</v>
@@ -18799,16 +18802,16 @@
       <c r="D5" s="28"/>
       <c r="I5" s="8"/>
       <c r="N5" s="21" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="O5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="P5" s="21" t="s">
         <v>41</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="R5" t="s">
         <v>59</v>
@@ -18821,19 +18824,19 @@
       <c r="D6" s="28"/>
       <c r="I6" s="8"/>
       <c r="N6" s="21" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="O6" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Q6" s="21" t="s">
         <v>34</v>
       </c>
       <c r="R6" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="S6" s="31" t="s">
         <v>60</v>
@@ -18843,16 +18846,16 @@
       <c r="D7" s="8"/>
       <c r="I7" s="8"/>
       <c r="N7" s="21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="O7" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="P7" s="21" t="s">
         <v>46</v>
       </c>
       <c r="Q7" s="21" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="R7" t="s">
         <v>64</v>
@@ -18864,16 +18867,16 @@
     <row r="8" spans="1:34">
       <c r="I8" s="8"/>
       <c r="N8" s="21" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="O8" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="Q8" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R8" t="s">
         <v>65</v>
@@ -18886,16 +18889,16 @@
       <c r="D9" s="8"/>
       <c r="I9" s="8"/>
       <c r="N9" s="21" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="O9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="P9" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q9" s="21" t="s">
         <v>268</v>
-      </c>
-      <c r="Q9" s="21" t="s">
-        <v>272</v>
       </c>
       <c r="R9" t="s">
         <v>66</v>
@@ -18907,229 +18910,229 @@
     <row r="10" spans="1:34">
       <c r="I10" s="8"/>
       <c r="N10" s="21" t="s">
-        <v>537</v>
+        <v>521</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="Q10" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R10" s="21" t="s">
-        <v>546</v>
+        <v>530</v>
       </c>
       <c r="S10" s="46" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="11" spans="1:34">
       <c r="I11" s="8"/>
       <c r="N11" s="21" t="s">
-        <v>538</v>
+        <v>522</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="Q11" s="21" t="s">
         <v>42</v>
       </c>
       <c r="R11" s="21" t="s">
-        <v>547</v>
+        <v>531</v>
       </c>
       <c r="S11" s="46" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="12" spans="1:34">
       <c r="I12" s="8"/>
       <c r="N12" s="21" t="s">
-        <v>539</v>
+        <v>523</v>
       </c>
       <c r="O12" s="21" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="P12" s="21" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="Q12" s="21" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="R12" s="21" t="s">
-        <v>548</v>
+        <v>532</v>
       </c>
       <c r="S12" s="46" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="13" spans="1:34">
       <c r="I13" s="8"/>
       <c r="N13" s="21" t="s">
-        <v>540</v>
+        <v>524</v>
       </c>
       <c r="O13" s="21" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="P13" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Q13" s="21" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="R13" s="21" t="s">
-        <v>549</v>
+        <v>533</v>
       </c>
       <c r="S13" s="46" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="14" spans="1:34">
       <c r="I14" s="8"/>
       <c r="N14" s="21" t="s">
-        <v>542</v>
+        <v>526</v>
       </c>
       <c r="O14" s="21" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="P14" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="Q14" s="21" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="R14" s="21" t="s">
-        <v>550</v>
+        <v>534</v>
       </c>
       <c r="S14" s="46" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="15" spans="1:34">
       <c r="I15" s="8"/>
       <c r="N15" s="21" t="s">
-        <v>541</v>
+        <v>525</v>
       </c>
       <c r="O15" s="21" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="Q15" s="21" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="R15" s="21" t="s">
-        <v>551</v>
+        <v>535</v>
       </c>
       <c r="S15" s="46" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="16" spans="1:34">
       <c r="I16" s="8"/>
       <c r="N16" s="21" t="s">
-        <v>543</v>
+        <v>527</v>
       </c>
       <c r="O16" s="21" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="P16" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="Q16" s="21" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="R16" s="21" t="s">
-        <v>552</v>
+        <v>536</v>
       </c>
       <c r="S16" s="46" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="17" spans="9:19">
       <c r="I17" s="8"/>
       <c r="N17" s="21" t="s">
-        <v>544</v>
+        <v>528</v>
       </c>
       <c r="O17" s="21" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="P17" s="21" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="Q17" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R17" s="21" t="s">
-        <v>553</v>
+        <v>537</v>
       </c>
       <c r="S17" s="46" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="18" spans="9:19">
       <c r="I18" s="8"/>
       <c r="N18" s="21" t="s">
-        <v>545</v>
+        <v>529</v>
       </c>
       <c r="O18" s="21" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="P18" s="21" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="Q18" s="21" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="R18" s="21" t="s">
-        <v>554</v>
+        <v>538</v>
       </c>
       <c r="S18" s="46" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="19" spans="9:19">
       <c r="I19" s="8"/>
       <c r="N19" s="21" t="s">
-        <v>555</v>
+        <v>539</v>
       </c>
       <c r="O19" s="21" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="P19" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Q19" s="21" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="R19" s="21" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="S19" s="46" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="20" spans="9:19">
       <c r="I20" s="8"/>
       <c r="N20" t="s">
-        <v>521</v>
+        <v>505</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>522</v>
+        <v>506</v>
       </c>
       <c r="P20" s="21" t="s">
         <v>42</v>
       </c>
       <c r="Q20" s="21" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="R20" s="66" t="s">
-        <v>523</v>
+        <v>507</v>
       </c>
       <c r="S20" s="31" t="s">
         <v>232</v>
@@ -19138,19 +19141,19 @@
     <row r="21" spans="9:19">
       <c r="I21" s="8"/>
       <c r="N21" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
       <c r="P21" s="21" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="Q21" s="21" t="s">
-        <v>528</v>
+        <v>512</v>
       </c>
       <c r="R21" s="66" t="s">
-        <v>529</v>
+        <v>513</v>
       </c>
       <c r="S21" s="31" t="s">
         <v>232</v>
@@ -19159,19 +19162,19 @@
     <row r="22" spans="9:19">
       <c r="I22" s="8"/>
       <c r="N22" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="O22" s="21" t="s">
-        <v>527</v>
+        <v>511</v>
       </c>
       <c r="P22" s="21" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="Q22" s="21" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="R22" s="66" t="s">
-        <v>530</v>
+        <v>514</v>
       </c>
       <c r="S22" s="31" t="s">
         <v>232</v>
@@ -19180,7 +19183,7 @@
     <row r="23" spans="9:19">
       <c r="I23" s="8"/>
       <c r="J23" s="28" t="s">
-        <v>519</v>
+        <v>541</v>
       </c>
       <c r="K23" s="28">
         <v>1472307</v>
@@ -19192,7 +19195,7 @@
         <v>42</v>
       </c>
       <c r="R23" t="s">
-        <v>520</v>
+        <v>504</v>
       </c>
       <c r="S23" s="31" t="s">
         <v>232</v>
@@ -19201,7 +19204,7 @@
     <row r="24" spans="9:19">
       <c r="I24" s="8"/>
       <c r="J24" s="28" t="s">
-        <v>515</v>
+        <v>542</v>
       </c>
       <c r="K24" s="28">
         <v>1472358</v>
@@ -19213,7 +19216,7 @@
         <v>42</v>
       </c>
       <c r="R24" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
       <c r="S24" s="31" t="s">
         <v>232</v>
@@ -19222,7 +19225,7 @@
     <row r="25" spans="9:19">
       <c r="I25" s="8"/>
       <c r="J25" s="28" t="s">
-        <v>511</v>
+        <v>543</v>
       </c>
       <c r="K25" s="28">
         <v>1472359</v>
@@ -19234,7 +19237,7 @@
         <v>45</v>
       </c>
       <c r="R25" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="S25" s="31" t="s">
         <v>232</v>
@@ -19243,7 +19246,7 @@
     <row r="26" spans="9:19">
       <c r="I26" s="8"/>
       <c r="J26" s="28" t="s">
-        <v>512</v>
+        <v>544</v>
       </c>
       <c r="K26" s="28">
         <v>1472359</v>
@@ -19255,7 +19258,7 @@
         <v>42</v>
       </c>
       <c r="R26" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="S26" s="31" t="s">
         <v>232</v>
@@ -19264,7 +19267,7 @@
     <row r="27" spans="9:19">
       <c r="I27" s="8"/>
       <c r="J27" s="28" t="s">
-        <v>517</v>
+        <v>545</v>
       </c>
       <c r="K27" s="28">
         <v>1472362</v>
@@ -19276,7 +19279,7 @@
         <v>42</v>
       </c>
       <c r="R27" t="s">
-        <v>518</v>
+        <v>503</v>
       </c>
       <c r="S27" s="31" t="s">
         <v>232</v>
@@ -19285,7 +19288,7 @@
     <row r="28" spans="9:19">
       <c r="I28" s="8"/>
       <c r="J28" s="28" t="s">
-        <v>508</v>
+        <v>546</v>
       </c>
       <c r="K28" s="28">
         <v>1473246</v>
@@ -19306,7 +19309,7 @@
     <row r="29" spans="9:19">
       <c r="I29" s="8"/>
       <c r="J29" s="28" t="s">
-        <v>509</v>
+        <v>547</v>
       </c>
       <c r="K29" s="28">
         <v>1473247</v>
@@ -19327,7 +19330,7 @@
     <row r="30" spans="9:19">
       <c r="I30" s="8"/>
       <c r="J30" s="28" t="s">
-        <v>510</v>
+        <v>548</v>
       </c>
       <c r="K30" s="28">
         <v>1473329</v>
@@ -19348,7 +19351,7 @@
     <row r="31" spans="9:19">
       <c r="I31" s="8"/>
       <c r="J31" s="35" t="s">
-        <v>285</v>
+        <v>549</v>
       </c>
       <c r="K31" s="28">
         <v>1673425</v>
@@ -19369,19 +19372,19 @@
     <row r="32" spans="9:19">
       <c r="I32" s="8"/>
       <c r="N32" t="s">
-        <v>531</v>
+        <v>515</v>
       </c>
       <c r="O32" s="21" t="s">
-        <v>532</v>
+        <v>516</v>
       </c>
       <c r="P32" s="21" t="s">
         <v>34</v>
       </c>
       <c r="Q32" s="21" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="R32" s="66" t="s">
-        <v>533</v>
+        <v>517</v>
       </c>
       <c r="S32" s="31" t="s">
         <v>128</v>
@@ -19390,19 +19393,19 @@
     <row r="33" spans="9:19">
       <c r="I33" s="8"/>
       <c r="N33" s="21" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="O33" s="21" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="P33" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="Q33" s="21" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="R33" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="S33" s="31" t="s">
         <v>43</v>
@@ -19410,8 +19413,8 @@
     </row>
     <row r="34" spans="9:19">
       <c r="I34" s="8"/>
-      <c r="J34" s="46" t="s">
-        <v>367</v>
+      <c r="J34" s="80" t="s">
+        <v>550</v>
       </c>
       <c r="K34" s="67">
         <v>2289248</v>
@@ -19426,7 +19429,7 @@
       <c r="P34" s="21"/>
       <c r="Q34" s="21"/>
       <c r="R34" s="66" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="S34" s="46" t="s">
         <v>36</v>
@@ -19434,8 +19437,8 @@
     </row>
     <row r="35" spans="9:19">
       <c r="I35" s="8"/>
-      <c r="J35" s="46" t="s">
-        <v>289</v>
+      <c r="J35" s="80" t="s">
+        <v>551</v>
       </c>
       <c r="K35" s="67">
         <v>2289252</v>
@@ -19450,7 +19453,7 @@
       <c r="P35" s="21"/>
       <c r="Q35" s="21"/>
       <c r="R35" s="66" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="S35" s="46" t="s">
         <v>36</v>
@@ -19458,8 +19461,8 @@
     </row>
     <row r="36" spans="9:19">
       <c r="I36" s="8"/>
-      <c r="J36" s="46" t="s">
-        <v>368</v>
+      <c r="J36" s="80" t="s">
+        <v>552</v>
       </c>
       <c r="K36" s="67">
         <v>2289253</v>
@@ -19474,7 +19477,7 @@
       <c r="P36" s="21"/>
       <c r="Q36" s="21"/>
       <c r="R36" s="66" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="S36" s="46" t="s">
         <v>36</v>
@@ -19487,19 +19490,19 @@
       <c r="L37" s="38"/>
       <c r="M37" s="38"/>
       <c r="N37" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="O37" s="21" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="P37" s="21" t="s">
         <v>46</v>
       </c>
       <c r="Q37" s="21" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="R37" s="66" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="S37" s="46" t="s">
         <v>36</v>
@@ -19512,19 +19515,19 @@
       <c r="L38" s="38"/>
       <c r="M38" s="38"/>
       <c r="N38" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="O38" s="21" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="P38" s="21" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="Q38" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="R38" s="66" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="S38" s="46" t="s">
         <v>36</v>
@@ -19537,19 +19540,19 @@
       <c r="L39" s="38"/>
       <c r="M39" s="38"/>
       <c r="N39" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="O39" s="21" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="P39" s="21" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="Q39" s="21" t="s">
         <v>42</v>
       </c>
       <c r="R39" s="66" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="S39" s="46" t="s">
         <v>36</v>
@@ -19562,19 +19565,19 @@
       <c r="L40" s="38"/>
       <c r="M40" s="38"/>
       <c r="N40" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="O40" s="21" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="Q40" s="21" t="s">
         <v>41</v>
       </c>
       <c r="R40" s="66" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="S40" s="46" t="s">
         <v>36</v>
@@ -19587,19 +19590,19 @@
       <c r="L41" s="38"/>
       <c r="M41" s="38"/>
       <c r="N41" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="O41" s="21" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="P41" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Q41" s="21" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="R41" s="66" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="S41" s="46" t="s">
         <v>36</v>
@@ -19612,19 +19615,19 @@
       <c r="L42" s="38"/>
       <c r="M42" s="38"/>
       <c r="N42" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="O42" s="21" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="Q42" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R42" s="66" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="S42" s="46" t="s">
         <v>36</v>
@@ -19637,19 +19640,19 @@
       <c r="L43" s="38"/>
       <c r="M43" s="38"/>
       <c r="N43" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="O43" s="21" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="P43" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Q43" s="21" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="R43" s="66" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="S43" s="46" t="s">
         <v>36</v>
@@ -19662,19 +19665,19 @@
       <c r="L44" s="38"/>
       <c r="M44" s="38"/>
       <c r="N44" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="O44" s="21" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="P44" s="21" t="s">
         <v>45</v>
       </c>
       <c r="Q44" s="21" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="R44" s="66" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="S44" s="46" t="s">
         <v>36</v>
@@ -19687,19 +19690,19 @@
       <c r="L45" s="38"/>
       <c r="M45" s="38"/>
       <c r="N45" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="O45" s="21" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="P45" s="21" t="s">
         <v>41</v>
       </c>
       <c r="Q45" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="R45" s="66" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="S45" s="46" t="s">
         <v>36</v>
@@ -19712,19 +19715,19 @@
       <c r="L46" s="38"/>
       <c r="M46" s="38"/>
       <c r="N46" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="O46" s="21" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="P46" s="21" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="Q46" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R46" s="66" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="S46" s="46" t="s">
         <v>36</v>
@@ -19737,19 +19740,19 @@
       <c r="L47" s="38"/>
       <c r="M47" s="38"/>
       <c r="N47" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="O47" s="21" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="P47" s="21" t="s">
         <v>41</v>
       </c>
       <c r="Q47" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="R47" s="66" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="S47" s="46" t="s">
         <v>36</v>
@@ -19762,19 +19765,19 @@
       <c r="L48" s="38"/>
       <c r="M48" s="38"/>
       <c r="N48" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="O48" s="21" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="P48" s="21" t="s">
         <v>131</v>
       </c>
       <c r="Q48" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="R48" s="66" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="S48" s="46" t="s">
         <v>36</v>
@@ -19787,19 +19790,19 @@
       <c r="L49" s="38"/>
       <c r="M49" s="38"/>
       <c r="N49" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="O49" s="21" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="P49" s="21" t="s">
         <v>46</v>
       </c>
       <c r="Q49" s="21" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="R49" s="66" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="S49" s="46" t="s">
         <v>36</v>
@@ -19812,19 +19815,19 @@
       <c r="L50" s="38"/>
       <c r="M50" s="38"/>
       <c r="N50" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="O50" s="21" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="P50" s="21" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="Q50" s="21" t="s">
         <v>42</v>
       </c>
       <c r="R50" s="66" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="S50" s="46" t="s">
         <v>36</v>
@@ -19837,19 +19840,19 @@
       <c r="L51" s="38"/>
       <c r="M51" s="38"/>
       <c r="N51" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="O51" s="21" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="P51" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Q51" s="21" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="R51" s="66" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="S51" s="46" t="s">
         <v>36</v>
@@ -19862,19 +19865,19 @@
       <c r="L52" s="38"/>
       <c r="M52" s="38"/>
       <c r="N52" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="O52" s="21" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="Q52" s="21" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="R52" s="66" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="S52" s="46" t="s">
         <v>36</v>
@@ -19887,19 +19890,19 @@
       <c r="L53" s="38"/>
       <c r="M53" s="38"/>
       <c r="N53" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="O53" s="21" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="Q53" s="21" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="R53" s="66" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="S53" s="46" t="s">
         <v>36</v>
@@ -19912,19 +19915,19 @@
       <c r="L54" s="38"/>
       <c r="M54" s="38"/>
       <c r="N54" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="O54" s="21" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="P54" s="21" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="Q54" s="21" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="R54" s="66" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="S54" s="46" t="s">
         <v>36</v>
@@ -19937,19 +19940,19 @@
       <c r="L55" s="38"/>
       <c r="M55" s="38"/>
       <c r="N55" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="O55" s="21" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="P55" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="Q55" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R55" s="66" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="S55" s="46" t="s">
         <v>36</v>
@@ -19962,19 +19965,19 @@
       <c r="L56" s="38"/>
       <c r="M56" s="38"/>
       <c r="N56" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="O56" s="21" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="P56" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="Q56" s="21" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="R56" s="66" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="S56" s="46" t="s">
         <v>36</v>
@@ -19987,19 +19990,19 @@
       <c r="L57" s="38"/>
       <c r="M57" s="38"/>
       <c r="N57" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="O57" s="21" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="P57" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Q57" s="21" t="s">
         <v>41</v>
       </c>
       <c r="R57" s="66" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="S57" s="46" t="s">
         <v>36</v>
@@ -20012,19 +20015,19 @@
       <c r="L58" s="38"/>
       <c r="M58" s="38"/>
       <c r="N58" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="O58" s="21" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="P58" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="Q58" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R58" s="66" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="S58" s="46" t="s">
         <v>36</v>
@@ -20037,19 +20040,19 @@
       <c r="L59" s="38"/>
       <c r="M59" s="38"/>
       <c r="N59" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="O59" s="21" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="P59" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="Q59" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R59" s="66" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="S59" s="46" t="s">
         <v>36</v>
@@ -20062,19 +20065,19 @@
       <c r="L60" s="38"/>
       <c r="M60" s="38"/>
       <c r="N60" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="O60" s="21" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="P60" s="21" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="Q60" s="21" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="R60" s="66" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="S60" s="46" t="s">
         <v>36</v>
@@ -20087,19 +20090,19 @@
       <c r="L61" s="38"/>
       <c r="M61" s="38"/>
       <c r="N61" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="O61" s="21" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="P61" s="21" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="Q61" s="21" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="R61" s="66" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="S61" s="46" t="s">
         <v>36</v>
@@ -20113,19 +20116,19 @@
       <c r="L62" s="38"/>
       <c r="M62" s="38"/>
       <c r="N62" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="O62" s="21" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="P62" s="21" t="s">
         <v>45</v>
       </c>
       <c r="Q62" s="21" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="R62" s="66" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="S62" s="46" t="s">
         <v>36</v>
@@ -20139,19 +20142,19 @@
       <c r="L63" s="38"/>
       <c r="M63" s="38"/>
       <c r="N63" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="O63" s="21" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="P63" s="21" t="s">
         <v>42</v>
       </c>
       <c r="Q63" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R63" s="66" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="S63" s="46" t="s">
         <v>36</v>
@@ -20164,19 +20167,19 @@
       <c r="L64" s="38"/>
       <c r="M64" s="38"/>
       <c r="N64" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="O64" s="21" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="P64" s="21" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="Q64" s="21" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="R64" s="66" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="S64" s="46" t="s">
         <v>36</v>
@@ -20189,19 +20192,19 @@
       <c r="L65" s="38"/>
       <c r="M65" s="38"/>
       <c r="N65" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="O65" s="21" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="P65" s="21" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="Q65" s="21" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="R65" s="66" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="S65" s="46" t="s">
         <v>36</v>
@@ -20215,19 +20218,19 @@
       <c r="L66" s="38"/>
       <c r="M66" s="38"/>
       <c r="N66" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="O66" s="21" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="P66" s="21" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="Q66" s="21" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="R66" s="66" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="S66" s="46" t="s">
         <v>36</v>
@@ -20241,19 +20244,19 @@
       <c r="L67" s="38"/>
       <c r="M67" s="38"/>
       <c r="N67" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="O67" s="21" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="P67" s="21" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="Q67" s="21" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="R67" s="66" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="S67" s="46" t="s">
         <v>36</v>
@@ -20267,19 +20270,19 @@
       <c r="L68" s="38"/>
       <c r="M68" s="38"/>
       <c r="N68" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="O68" s="21" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="P68" s="21" t="s">
         <v>41</v>
       </c>
       <c r="Q68" s="21" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="R68" s="66" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="S68" s="46" t="s">
         <v>36</v>
@@ -20293,19 +20296,19 @@
       <c r="L69" s="38"/>
       <c r="M69" s="38"/>
       <c r="N69" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="O69" s="21" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="P69" s="21" t="s">
         <v>131</v>
       </c>
       <c r="Q69" s="21" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="R69" s="66" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="S69" s="46" t="s">
         <v>36</v>
@@ -20319,19 +20322,19 @@
       <c r="L70" s="38"/>
       <c r="M70" s="38"/>
       <c r="N70" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="O70" s="21" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="P70" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="Q70" s="21" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="R70" s="66" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="S70" s="46" t="s">
         <v>36</v>
@@ -20344,19 +20347,19 @@
       <c r="L71" s="38"/>
       <c r="M71" s="38"/>
       <c r="N71" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="O71" s="21" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="P71" s="21" t="s">
         <v>41</v>
       </c>
       <c r="Q71" s="21" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="R71" s="66" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="S71" s="46" t="s">
         <v>36</v>
@@ -20369,19 +20372,19 @@
       <c r="L72" s="38"/>
       <c r="M72" s="38"/>
       <c r="N72" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="O72" s="21" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="P72" s="21" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="Q72" s="21" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="R72" s="66" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="S72" s="46" t="s">
         <v>36</v>
@@ -20394,19 +20397,19 @@
       <c r="L73" s="38"/>
       <c r="M73" s="38"/>
       <c r="N73" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="O73" s="21" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="P73" s="21" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="Q73" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R73" s="66" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="S73" s="46" t="s">
         <v>36</v>
@@ -20419,19 +20422,19 @@
       <c r="L74" s="38"/>
       <c r="M74" s="38"/>
       <c r="N74" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="O74" s="21" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="P74" s="21" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="Q74" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R74" s="66" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="S74" s="46" t="s">
         <v>36</v>
@@ -20444,19 +20447,19 @@
       <c r="L75" s="38"/>
       <c r="M75" s="38"/>
       <c r="N75" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="O75" s="21" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="P75" s="21" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="Q75" s="21" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="R75" s="66" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="S75" s="46" t="s">
         <v>36</v>
@@ -20469,19 +20472,19 @@
       <c r="L76" s="38"/>
       <c r="M76" s="38"/>
       <c r="N76" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="O76" s="21" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="P76" s="21" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="Q76" s="21" t="s">
         <v>41</v>
       </c>
       <c r="R76" s="66" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="S76" s="46" t="s">
         <v>36</v>
@@ -20494,19 +20497,19 @@
       <c r="L77" s="38"/>
       <c r="M77" s="38"/>
       <c r="N77" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="O77" s="21" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="P77" s="21" t="s">
         <v>41</v>
       </c>
       <c r="Q77" s="21" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="R77" s="66" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="S77" s="46" t="s">
         <v>36</v>
@@ -20519,19 +20522,19 @@
       <c r="L78" s="38"/>
       <c r="M78" s="38"/>
       <c r="N78" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="O78" s="21" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="P78" s="21" t="s">
         <v>46</v>
       </c>
       <c r="Q78" s="21" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="R78" s="66" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="S78" s="46" t="s">
         <v>36</v>
@@ -20544,19 +20547,19 @@
       <c r="L79" s="38"/>
       <c r="M79" s="38"/>
       <c r="N79" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="O79" s="21" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="P79" s="21" t="s">
         <v>42</v>
       </c>
       <c r="Q79" s="21" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="R79" s="66" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="S79" s="46" t="s">
         <v>36</v>
@@ -20569,19 +20572,19 @@
       <c r="L80" s="38"/>
       <c r="M80" s="38"/>
       <c r="N80" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="O80" s="21" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="P80" s="21" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="Q80" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R80" s="66" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="S80" s="46" t="s">
         <v>36</v>
@@ -20594,10 +20597,10 @@
       <c r="L81" s="38"/>
       <c r="M81" s="38"/>
       <c r="N81" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="O81" s="21" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="P81" s="21" t="s">
         <v>45</v>
@@ -20606,7 +20609,7 @@
         <v>131</v>
       </c>
       <c r="R81" s="66" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="S81" s="46" t="s">
         <v>36</v>
@@ -20619,19 +20622,19 @@
       <c r="L82" s="38"/>
       <c r="M82" s="38"/>
       <c r="N82" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="O82" s="21" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="P82" s="21" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="Q82" s="21" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="R82" s="66" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="S82" s="46" t="s">
         <v>36</v>
@@ -20644,19 +20647,19 @@
       <c r="L83" s="38"/>
       <c r="M83" s="38"/>
       <c r="N83" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="O83" s="21" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="P83" s="21" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="Q83" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R83" s="66" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="S83" s="46" t="s">
         <v>36</v>
@@ -20669,19 +20672,19 @@
       <c r="L84" s="38"/>
       <c r="M84" s="38"/>
       <c r="N84" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="O84" s="21" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="P84" s="21" t="s">
         <v>42</v>
       </c>
       <c r="Q84" s="21" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="R84" s="66" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="S84" s="46" t="s">
         <v>36</v>
@@ -20694,19 +20697,19 @@
       <c r="L85" s="38"/>
       <c r="M85" s="38"/>
       <c r="N85" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="O85" s="21" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="P85" s="21" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="Q85" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="R85" s="66" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="S85" s="46" t="s">
         <v>36</v>
@@ -20720,19 +20723,19 @@
       <c r="L86" s="38"/>
       <c r="M86" s="38"/>
       <c r="N86" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="O86" s="21" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="P86" s="21" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="Q86" s="21" t="s">
         <v>41</v>
       </c>
       <c r="R86" s="66" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="S86" s="46" t="s">
         <v>36</v>
@@ -20747,19 +20750,19 @@
       <c r="L87" s="38"/>
       <c r="M87" s="38"/>
       <c r="N87" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="O87" s="21" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="P87" s="21" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="Q87" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R87" s="66" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="S87" s="46" t="s">
         <v>36</v>
@@ -20774,19 +20777,19 @@
       <c r="L88" s="38"/>
       <c r="M88" s="38"/>
       <c r="N88" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="O88" s="21" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="P88" s="21" t="s">
         <v>42</v>
       </c>
       <c r="Q88" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R88" s="66" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="S88" s="46" t="s">
         <v>36</v>
@@ -20801,19 +20804,19 @@
       <c r="L89" s="38"/>
       <c r="M89" s="38"/>
       <c r="N89" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="O89" s="21" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="P89" s="21" t="s">
         <v>41</v>
       </c>
       <c r="Q89" s="21" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="R89" s="66" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="S89" s="46" t="s">
         <v>36</v>
@@ -20828,19 +20831,19 @@
       <c r="L90" s="38"/>
       <c r="M90" s="38"/>
       <c r="N90" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="O90" s="21" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="P90" s="21" t="s">
         <v>42</v>
       </c>
       <c r="Q90" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R90" s="66" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="S90" s="46" t="s">
         <v>36</v>
@@ -20855,19 +20858,19 @@
       <c r="L91" s="38"/>
       <c r="M91" s="38"/>
       <c r="N91" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="O91" s="21" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="P91" s="21" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="Q91" s="21" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="R91" s="66" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="S91" s="46" t="s">
         <v>36</v>
@@ -20880,19 +20883,19 @@
       <c r="L92" s="38"/>
       <c r="M92" s="38"/>
       <c r="N92" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="O92" s="21" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="P92" s="21" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="Q92" s="21" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="R92" s="66" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="S92" s="46" t="s">
         <v>36</v>
@@ -20906,19 +20909,19 @@
       <c r="L93" s="38"/>
       <c r="M93" s="38"/>
       <c r="N93" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="O93" s="21" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="P93" s="21" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="Q93" s="21" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="R93" s="66" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="S93" s="46" t="s">
         <v>36</v>
@@ -20928,7 +20931,7 @@
     <row r="94" spans="4:20">
       <c r="I94" s="8"/>
       <c r="J94" s="35" t="s">
-        <v>258</v>
+        <v>553</v>
       </c>
       <c r="K94" s="36">
         <v>2715342</v>
@@ -20950,7 +20953,7 @@
       <c r="D95" s="8"/>
       <c r="I95" s="8"/>
       <c r="J95" s="35" t="s">
-        <v>259</v>
+        <v>554</v>
       </c>
       <c r="K95" s="36">
         <v>2715344</v>
@@ -20972,7 +20975,7 @@
       <c r="D96" s="8"/>
       <c r="I96" s="10"/>
       <c r="J96" s="37" t="s">
-        <v>260</v>
+        <v>555</v>
       </c>
       <c r="K96" s="36">
         <v>2715346</v>
@@ -20993,7 +20996,7 @@
     <row r="97" spans="1:32">
       <c r="I97" s="8"/>
       <c r="J97" s="35" t="s">
-        <v>261</v>
+        <v>556</v>
       </c>
       <c r="K97" s="36">
         <v>2715369</v>

</xml_diff>

<commit_message>
Updates to TB whole genome reference json file
</commit_message>
<xml_diff>
--- a/assay_data/TB_assays.xlsx
+++ b/assay_data/TB_assays.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="3860" windowWidth="38400" windowHeight="21960" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="24860" yWindow="5220" windowWidth="38400" windowHeight="21960" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TB" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="563">
   <si>
     <t>Assay Name</t>
   </si>
@@ -2388,9 +2388,6 @@
     <t>pncA V180 mutation present which is associated with pyrazinamide resistance.</t>
   </si>
   <si>
-    <t>K,L,P</t>
-  </si>
-  <si>
     <t>Q,L</t>
   </si>
   <si>
@@ -2416,9 +2413,6 @@
   </si>
   <si>
     <t>761127-761129</t>
-  </si>
-  <si>
-    <t>C,D,F,G,L,N,R,Y</t>
   </si>
   <si>
     <t>761139-761141</t>
@@ -2703,6 +2697,30 @@
   </si>
   <si>
     <t>-37G&gt;T</t>
+  </si>
+  <si>
+    <t>F424</t>
+  </si>
+  <si>
+    <t>761076-761078</t>
+  </si>
+  <si>
+    <t>H,K,L,P</t>
+  </si>
+  <si>
+    <t>rpoB F424V (F505V) mutation present which is associated with rifampicin resistance.</t>
+  </si>
+  <si>
+    <t>M434</t>
+  </si>
+  <si>
+    <t>761106-761108</t>
+  </si>
+  <si>
+    <t>C,D,F,G,L,N,P,R,Y</t>
+  </si>
+  <si>
+    <t>rpoB M434I (M515I) mutation present which is associated with rifampicin resistance.</t>
   </si>
 </sst>
 </file>
@@ -2961,7 +2979,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="449">
+  <cellStyleXfs count="453">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3268,6 +3286,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3571,6 +3593,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3607,11 +3632,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="449">
+  <cellStyles count="453">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -3969,6 +3991,8 @@
     <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -4059,6 +4083,8 @@
     <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25" customBuiltin="1"/>
   </cellStyles>
@@ -4419,37 +4445,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="1" customFormat="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="71" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="70" t="s">
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="70"/>
-      <c r="J1" s="71" t="s">
+      <c r="I1" s="71"/>
+      <c r="J1" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="71" t="s">
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="68" t="s">
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="69"/>
+      <c r="S1" s="70"/>
       <c r="AD1" s="23" t="s">
         <v>19</v>
       </c>
@@ -9712,37 +9738,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="1" customFormat="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="71" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="70" t="s">
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="70"/>
-      <c r="J1" s="71" t="s">
+      <c r="I1" s="71"/>
+      <c r="J1" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="71" t="s">
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="68" t="s">
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="69"/>
+      <c r="S1" s="70"/>
       <c r="AD1" s="23" t="s">
         <v>19</v>
       </c>
@@ -15057,37 +15083,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="38" customFormat="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="77" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="76" t="s">
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="76"/>
-      <c r="J1" s="77" t="s">
+      <c r="I1" s="77"/>
+      <c r="J1" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="77" t="s">
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="74" t="s">
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="75"/>
+      <c r="S1" s="76"/>
       <c r="AD1" s="64" t="s">
         <v>19</v>
       </c>
@@ -18597,10 +18623,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH724"/>
+  <dimension ref="A1:AH726"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J98" sqref="J98"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18627,37 +18653,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="1" customFormat="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="71" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="70" t="s">
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="70"/>
-      <c r="J1" s="71" t="s">
+      <c r="I1" s="71"/>
+      <c r="J1" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="71" t="s">
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="68" t="s">
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="69"/>
+      <c r="S1" s="70"/>
       <c r="AD1" s="23" t="s">
         <v>19</v>
       </c>
@@ -18756,10 +18782,10 @@
         <v>25</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="N3" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="O3" t="s">
         <v>277</v>
@@ -18780,7 +18806,7 @@
     <row r="4" spans="1:34">
       <c r="I4" s="8"/>
       <c r="N4" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="O4" t="s">
         <v>278</v>
@@ -18910,271 +18936,271 @@
     <row r="10" spans="1:34">
       <c r="I10" s="8"/>
       <c r="N10" s="21" t="s">
-        <v>521</v>
+        <v>555</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>487</v>
+        <v>556</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
       <c r="Q10" s="21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="R10" s="21" t="s">
-        <v>530</v>
+        <v>558</v>
       </c>
       <c r="S10" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:34">
       <c r="I11" s="8"/>
       <c r="N11" s="21" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>266</v>
+        <v>311</v>
       </c>
       <c r="Q11" s="21" t="s">
-        <v>42</v>
+        <v>267</v>
       </c>
       <c r="R11" s="21" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="S11" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="12" spans="1:34">
       <c r="I12" s="8"/>
       <c r="N12" s="21" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="O12" s="21" t="s">
         <v>488</v>
       </c>
       <c r="P12" s="21" t="s">
-        <v>294</v>
+        <v>266</v>
       </c>
       <c r="Q12" s="21" t="s">
-        <v>483</v>
+        <v>42</v>
       </c>
       <c r="R12" s="21" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="S12" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="13" spans="1:34">
       <c r="I13" s="8"/>
       <c r="N13" s="21" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="O13" s="21" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="P13" s="21" t="s">
-        <v>264</v>
+        <v>294</v>
       </c>
       <c r="Q13" s="21" t="s">
-        <v>490</v>
+        <v>557</v>
       </c>
       <c r="R13" s="21" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="S13" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="14" spans="1:34">
       <c r="I14" s="8"/>
       <c r="N14" s="21" t="s">
-        <v>526</v>
+        <v>559</v>
       </c>
       <c r="O14" s="21" t="s">
-        <v>492</v>
+        <v>560</v>
       </c>
       <c r="P14" s="21" t="s">
-        <v>266</v>
+        <v>358</v>
       </c>
       <c r="Q14" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="R14" s="21" t="s">
+        <v>562</v>
+      </c>
+      <c r="S14" s="46" t="s">
         <v>484</v>
-      </c>
-      <c r="R14" s="21" t="s">
-        <v>534</v>
-      </c>
-      <c r="S14" s="46" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="15" spans="1:34">
       <c r="I15" s="8"/>
       <c r="N15" s="21" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="O15" s="21" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>309</v>
+        <v>264</v>
       </c>
       <c r="Q15" s="21" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="R15" s="21" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="S15" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="16" spans="1:34">
       <c r="I16" s="8"/>
       <c r="N16" s="21" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="O16" s="21" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="P16" s="21" t="s">
         <v>266</v>
       </c>
       <c r="Q16" s="21" t="s">
-        <v>495</v>
+        <v>483</v>
       </c>
       <c r="R16" s="21" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="S16" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="17" spans="9:19">
       <c r="I17" s="8"/>
       <c r="N17" s="21" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="O17" s="21" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="P17" s="21" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="Q17" s="21" t="s">
-        <v>267</v>
+        <v>561</v>
       </c>
       <c r="R17" s="21" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="S17" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="18" spans="9:19">
       <c r="I18" s="8"/>
       <c r="N18" s="21" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="O18" s="21" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="P18" s="21" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
       <c r="Q18" s="21" t="s">
-        <v>330</v>
+        <v>493</v>
       </c>
       <c r="R18" s="21" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="S18" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="19" spans="9:19">
       <c r="I19" s="8"/>
       <c r="N19" s="21" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="O19" s="21" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="P19" s="21" t="s">
-        <v>264</v>
+        <v>311</v>
       </c>
       <c r="Q19" s="21" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="R19" s="21" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="S19" s="46" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="20" spans="9:19">
       <c r="I20" s="8"/>
-      <c r="N20" t="s">
-        <v>505</v>
+      <c r="N20" s="21" t="s">
+        <v>527</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>506</v>
+        <v>496</v>
       </c>
       <c r="P20" s="21" t="s">
-        <v>42</v>
+        <v>288</v>
       </c>
       <c r="Q20" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="R20" s="66" t="s">
-        <v>507</v>
-      </c>
-      <c r="S20" s="31" t="s">
-        <v>232</v>
+        <v>330</v>
+      </c>
+      <c r="R20" s="21" t="s">
+        <v>536</v>
+      </c>
+      <c r="S20" s="46" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="9:19">
       <c r="I21" s="8"/>
-      <c r="N21" t="s">
-        <v>508</v>
+      <c r="N21" s="21" t="s">
+        <v>537</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="P21" s="21" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="Q21" s="21" t="s">
-        <v>512</v>
-      </c>
-      <c r="R21" s="66" t="s">
-        <v>513</v>
-      </c>
-      <c r="S21" s="31" t="s">
-        <v>232</v>
+        <v>275</v>
+      </c>
+      <c r="R21" s="21" t="s">
+        <v>538</v>
+      </c>
+      <c r="S21" s="46" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="22" spans="9:19">
       <c r="I22" s="8"/>
       <c r="N22" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="O22" s="21" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="P22" s="21" t="s">
-        <v>276</v>
+        <v>42</v>
       </c>
       <c r="Q22" s="21" t="s">
-        <v>390</v>
+        <v>288</v>
       </c>
       <c r="R22" s="66" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
       <c r="S22" s="31" t="s">
         <v>232</v>
@@ -19182,20 +19208,20 @@
     </row>
     <row r="23" spans="9:19">
       <c r="I23" s="8"/>
-      <c r="J23" s="28" t="s">
-        <v>541</v>
-      </c>
-      <c r="K23" s="28">
-        <v>1472307</v>
-      </c>
-      <c r="L23" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="M23" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="R23" t="s">
-        <v>504</v>
+      <c r="N23" t="s">
+        <v>506</v>
+      </c>
+      <c r="O23" s="21" t="s">
+        <v>508</v>
+      </c>
+      <c r="P23" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q23" s="21" t="s">
+        <v>510</v>
+      </c>
+      <c r="R23" s="66" t="s">
+        <v>511</v>
       </c>
       <c r="S23" s="31" t="s">
         <v>232</v>
@@ -19203,20 +19229,20 @@
     </row>
     <row r="24" spans="9:19">
       <c r="I24" s="8"/>
-      <c r="J24" s="28" t="s">
-        <v>542</v>
-      </c>
-      <c r="K24" s="28">
-        <v>1472358</v>
-      </c>
-      <c r="L24" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="M24" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="R24" t="s">
-        <v>502</v>
+      <c r="N24" t="s">
+        <v>507</v>
+      </c>
+      <c r="O24" s="21" t="s">
+        <v>509</v>
+      </c>
+      <c r="P24" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q24" s="21" t="s">
+        <v>390</v>
+      </c>
+      <c r="R24" s="66" t="s">
+        <v>512</v>
       </c>
       <c r="S24" s="31" t="s">
         <v>232</v>
@@ -19225,19 +19251,19 @@
     <row r="25" spans="9:19">
       <c r="I25" s="8"/>
       <c r="J25" s="28" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="K25" s="28">
-        <v>1472359</v>
+        <v>1472307</v>
       </c>
       <c r="L25" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M25" s="28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="R25" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="S25" s="31" t="s">
         <v>232</v>
@@ -19246,13 +19272,13 @@
     <row r="26" spans="9:19">
       <c r="I26" s="8"/>
       <c r="J26" s="28" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="K26" s="28">
-        <v>1472359</v>
+        <v>1472358</v>
       </c>
       <c r="L26" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M26" s="28" t="s">
         <v>42</v>
@@ -19267,19 +19293,19 @@
     <row r="27" spans="9:19">
       <c r="I27" s="8"/>
       <c r="J27" s="28" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="K27" s="28">
-        <v>1472362</v>
+        <v>1472359</v>
       </c>
       <c r="L27" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="M27" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="M27" s="28" t="s">
-        <v>42</v>
-      </c>
       <c r="R27" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="S27" s="31" t="s">
         <v>232</v>
@@ -19288,31 +19314,31 @@
     <row r="28" spans="9:19">
       <c r="I28" s="8"/>
       <c r="J28" s="28" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="K28" s="28">
-        <v>1473246</v>
+        <v>1472359</v>
       </c>
       <c r="L28" s="28" t="s">
         <v>46</v>
       </c>
       <c r="M28" s="28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R28" t="s">
-        <v>123</v>
+        <v>498</v>
       </c>
       <c r="S28" s="31" t="s">
-        <v>127</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="9:19">
       <c r="I29" s="8"/>
       <c r="J29" s="28" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="K29" s="28">
-        <v>1473247</v>
+        <v>1472362</v>
       </c>
       <c r="L29" s="28" t="s">
         <v>45</v>
@@ -19321,40 +19347,40 @@
         <v>42</v>
       </c>
       <c r="R29" t="s">
-        <v>129</v>
+        <v>501</v>
       </c>
       <c r="S29" s="31" t="s">
-        <v>128</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="9:19">
       <c r="I30" s="8"/>
       <c r="J30" s="28" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="K30" s="28">
-        <v>1473329</v>
+        <v>1473246</v>
       </c>
       <c r="L30" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="M30" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="M30" s="28" t="s">
-        <v>42</v>
-      </c>
       <c r="R30" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="S30" s="31" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="9:19">
       <c r="I31" s="8"/>
-      <c r="J31" s="35" t="s">
-        <v>549</v>
+      <c r="J31" s="28" t="s">
+        <v>545</v>
       </c>
       <c r="K31" s="28">
-        <v>1673425</v>
+        <v>1473247</v>
       </c>
       <c r="L31" s="28" t="s">
         <v>45</v>
@@ -19363,49 +19389,49 @@
         <v>42</v>
       </c>
       <c r="R31" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="S31" s="31" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="9:19">
       <c r="I32" s="8"/>
-      <c r="N32" t="s">
-        <v>515</v>
-      </c>
-      <c r="O32" s="21" t="s">
-        <v>516</v>
-      </c>
-      <c r="P32" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q32" s="21" t="s">
-        <v>276</v>
-      </c>
-      <c r="R32" s="66" t="s">
-        <v>517</v>
+      <c r="J32" s="28" t="s">
+        <v>546</v>
+      </c>
+      <c r="K32" s="28">
+        <v>1473329</v>
+      </c>
+      <c r="L32" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="M32" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="R32" t="s">
+        <v>130</v>
       </c>
       <c r="S32" s="31" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="9:19">
       <c r="I33" s="8"/>
-      <c r="N33" s="21" t="s">
-        <v>281</v>
-      </c>
-      <c r="O33" s="21" t="s">
-        <v>282</v>
-      </c>
-      <c r="P33" s="21" t="s">
-        <v>266</v>
-      </c>
-      <c r="Q33" s="21" t="s">
-        <v>283</v>
+      <c r="J33" s="35" t="s">
+        <v>547</v>
+      </c>
+      <c r="K33" s="28">
+        <v>1673425</v>
+      </c>
+      <c r="L33" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="M33" s="28" t="s">
+        <v>42</v>
       </c>
       <c r="R33" t="s">
-        <v>486</v>
+        <v>95</v>
       </c>
       <c r="S33" s="31" t="s">
         <v>43</v>
@@ -19413,59 +19439,53 @@
     </row>
     <row r="34" spans="9:19">
       <c r="I34" s="8"/>
-      <c r="J34" s="80" t="s">
-        <v>550</v>
-      </c>
-      <c r="K34" s="67">
-        <v>2289248</v>
-      </c>
-      <c r="L34" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="M34" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="O34" s="21"/>
-      <c r="P34" s="21"/>
-      <c r="Q34" s="21"/>
+      <c r="N34" t="s">
+        <v>513</v>
+      </c>
+      <c r="O34" s="21" t="s">
+        <v>514</v>
+      </c>
+      <c r="P34" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q34" s="21" t="s">
+        <v>276</v>
+      </c>
       <c r="R34" s="66" t="s">
-        <v>361</v>
-      </c>
-      <c r="S34" s="46" t="s">
-        <v>36</v>
+        <v>515</v>
+      </c>
+      <c r="S34" s="31" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="9:19">
       <c r="I35" s="8"/>
-      <c r="J35" s="80" t="s">
-        <v>551</v>
-      </c>
-      <c r="K35" s="67">
-        <v>2289252</v>
-      </c>
-      <c r="L35" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="M35" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="O35" s="21"/>
-      <c r="P35" s="21"/>
-      <c r="Q35" s="21"/>
-      <c r="R35" s="66" t="s">
-        <v>284</v>
-      </c>
-      <c r="S35" s="46" t="s">
-        <v>36</v>
+      <c r="N35" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="O35" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="P35" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q35" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="R35" t="s">
+        <v>485</v>
+      </c>
+      <c r="S35" s="31" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="9:19">
       <c r="I36" s="8"/>
-      <c r="J36" s="80" t="s">
-        <v>552</v>
+      <c r="J36" s="68" t="s">
+        <v>548</v>
       </c>
       <c r="K36" s="67">
-        <v>2289253</v>
+        <v>2289248</v>
       </c>
       <c r="L36" s="46" t="s">
         <v>46</v>
@@ -19477,7 +19497,7 @@
       <c r="P36" s="21"/>
       <c r="Q36" s="21"/>
       <c r="R36" s="66" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="S36" s="46" t="s">
         <v>36</v>
@@ -19485,24 +19505,23 @@
     </row>
     <row r="37" spans="9:19">
       <c r="I37" s="8"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="38"/>
-      <c r="L37" s="38"/>
-      <c r="M37" s="38"/>
-      <c r="N37" t="s">
-        <v>285</v>
-      </c>
-      <c r="O37" s="21" t="s">
-        <v>360</v>
-      </c>
-      <c r="P37" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q37" s="21" t="s">
-        <v>275</v>
-      </c>
+      <c r="J37" s="68" t="s">
+        <v>549</v>
+      </c>
+      <c r="K37" s="67">
+        <v>2289252</v>
+      </c>
+      <c r="L37" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="M37" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="21"/>
       <c r="R37" s="66" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="S37" s="46" t="s">
         <v>36</v>
@@ -19510,24 +19529,23 @@
     </row>
     <row r="38" spans="9:19">
       <c r="I38" s="8"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
-      <c r="L38" s="38"/>
-      <c r="M38" s="38"/>
-      <c r="N38" t="s">
-        <v>363</v>
-      </c>
-      <c r="O38" s="21" t="s">
-        <v>364</v>
-      </c>
-      <c r="P38" s="21" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q38" s="21" t="s">
-        <v>266</v>
-      </c>
+      <c r="J38" s="68" t="s">
+        <v>550</v>
+      </c>
+      <c r="K38" s="67">
+        <v>2289253</v>
+      </c>
+      <c r="L38" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="M38" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21"/>
       <c r="R38" s="66" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="S38" s="46" t="s">
         <v>36</v>
@@ -19540,19 +19558,19 @@
       <c r="L39" s="38"/>
       <c r="M39" s="38"/>
       <c r="N39" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O39" s="21" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="P39" s="21" t="s">
-        <v>288</v>
+        <v>46</v>
       </c>
       <c r="Q39" s="21" t="s">
-        <v>42</v>
+        <v>275</v>
       </c>
       <c r="R39" s="66" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="S39" s="46" t="s">
         <v>36</v>
@@ -19565,19 +19583,19 @@
       <c r="L40" s="38"/>
       <c r="M40" s="38"/>
       <c r="N40" t="s">
-        <v>290</v>
+        <v>363</v>
       </c>
       <c r="O40" s="21" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>265</v>
+        <v>311</v>
       </c>
       <c r="Q40" s="21" t="s">
-        <v>41</v>
+        <v>266</v>
       </c>
       <c r="R40" s="66" t="s">
-        <v>291</v>
+        <v>365</v>
       </c>
       <c r="S40" s="46" t="s">
         <v>36</v>
@@ -19590,19 +19608,19 @@
       <c r="L41" s="38"/>
       <c r="M41" s="38"/>
       <c r="N41" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="O41" s="21" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="P41" s="21" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="Q41" s="21" t="s">
-        <v>372</v>
+        <v>42</v>
       </c>
       <c r="R41" s="66" t="s">
-        <v>373</v>
+        <v>289</v>
       </c>
       <c r="S41" s="46" t="s">
         <v>36</v>
@@ -19615,19 +19633,19 @@
       <c r="L42" s="38"/>
       <c r="M42" s="38"/>
       <c r="N42" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="O42" s="21" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>294</v>
+        <v>265</v>
       </c>
       <c r="Q42" s="21" t="s">
-        <v>267</v>
+        <v>41</v>
       </c>
       <c r="R42" s="66" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="S42" s="46" t="s">
         <v>36</v>
@@ -19640,19 +19658,19 @@
       <c r="L43" s="38"/>
       <c r="M43" s="38"/>
       <c r="N43" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="O43" s="21" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="P43" s="21" t="s">
         <v>264</v>
       </c>
       <c r="Q43" s="21" t="s">
-        <v>297</v>
+        <v>372</v>
       </c>
       <c r="R43" s="66" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S43" s="46" t="s">
         <v>36</v>
@@ -19665,19 +19683,19 @@
       <c r="L44" s="38"/>
       <c r="M44" s="38"/>
       <c r="N44" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="O44" s="21" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="P44" s="21" t="s">
-        <v>45</v>
+        <v>294</v>
       </c>
       <c r="Q44" s="21" t="s">
-        <v>299</v>
+        <v>267</v>
       </c>
       <c r="R44" s="66" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="S44" s="46" t="s">
         <v>36</v>
@@ -19690,19 +19708,19 @@
       <c r="L45" s="38"/>
       <c r="M45" s="38"/>
       <c r="N45" t="s">
-        <v>375</v>
+        <v>296</v>
       </c>
       <c r="O45" s="21" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="P45" s="21" t="s">
-        <v>41</v>
+        <v>264</v>
       </c>
       <c r="Q45" s="21" t="s">
-        <v>264</v>
+        <v>297</v>
       </c>
       <c r="R45" s="66" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="S45" s="46" t="s">
         <v>36</v>
@@ -19715,19 +19733,19 @@
       <c r="L46" s="38"/>
       <c r="M46" s="38"/>
       <c r="N46" t="s">
-        <v>380</v>
+        <v>298</v>
       </c>
       <c r="O46" s="21" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="P46" s="21" t="s">
-        <v>311</v>
+        <v>45</v>
       </c>
       <c r="Q46" s="21" t="s">
-        <v>267</v>
+        <v>299</v>
       </c>
       <c r="R46" s="66" t="s">
-        <v>378</v>
+        <v>300</v>
       </c>
       <c r="S46" s="46" t="s">
         <v>36</v>
@@ -19740,10 +19758,10 @@
       <c r="L47" s="38"/>
       <c r="M47" s="38"/>
       <c r="N47" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="O47" s="21" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="P47" s="21" t="s">
         <v>41</v>
@@ -19752,7 +19770,7 @@
         <v>264</v>
       </c>
       <c r="R47" s="66" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="S47" s="46" t="s">
         <v>36</v>
@@ -19765,19 +19783,19 @@
       <c r="L48" s="38"/>
       <c r="M48" s="38"/>
       <c r="N48" t="s">
-        <v>301</v>
+        <v>380</v>
       </c>
       <c r="O48" s="21" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="P48" s="21" t="s">
-        <v>131</v>
+        <v>311</v>
       </c>
       <c r="Q48" s="21" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="R48" s="66" t="s">
-        <v>302</v>
+        <v>378</v>
       </c>
       <c r="S48" s="46" t="s">
         <v>36</v>
@@ -19790,19 +19808,19 @@
       <c r="L49" s="38"/>
       <c r="M49" s="38"/>
       <c r="N49" t="s">
-        <v>303</v>
+        <v>381</v>
       </c>
       <c r="O49" s="21" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="P49" s="21" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="Q49" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="R49" s="66" t="s">
-        <v>304</v>
+        <v>382</v>
       </c>
       <c r="S49" s="46" t="s">
         <v>36</v>
@@ -19815,19 +19833,19 @@
       <c r="L50" s="38"/>
       <c r="M50" s="38"/>
       <c r="N50" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="O50" s="21" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="P50" s="21" t="s">
-        <v>276</v>
+        <v>131</v>
       </c>
       <c r="Q50" s="21" t="s">
-        <v>42</v>
+        <v>264</v>
       </c>
       <c r="R50" s="66" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="S50" s="46" t="s">
         <v>36</v>
@@ -19840,19 +19858,19 @@
       <c r="L51" s="38"/>
       <c r="M51" s="38"/>
       <c r="N51" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="O51" s="21" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="P51" s="21" t="s">
-        <v>264</v>
+        <v>46</v>
       </c>
       <c r="Q51" s="21" t="s">
-        <v>388</v>
+        <v>265</v>
       </c>
       <c r="R51" s="66" t="s">
-        <v>389</v>
+        <v>304</v>
       </c>
       <c r="S51" s="46" t="s">
         <v>36</v>
@@ -19865,19 +19883,19 @@
       <c r="L52" s="38"/>
       <c r="M52" s="38"/>
       <c r="N52" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="O52" s="21" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="Q52" s="21" t="s">
-        <v>390</v>
+        <v>42</v>
       </c>
       <c r="R52" s="66" t="s">
-        <v>391</v>
+        <v>306</v>
       </c>
       <c r="S52" s="46" t="s">
         <v>36</v>
@@ -19890,19 +19908,19 @@
       <c r="L53" s="38"/>
       <c r="M53" s="38"/>
       <c r="N53" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="O53" s="21" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="P53" s="21" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="Q53" s="21" t="s">
-        <v>331</v>
+        <v>388</v>
       </c>
       <c r="R53" s="66" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="S53" s="46" t="s">
         <v>36</v>
@@ -19915,19 +19933,19 @@
       <c r="L54" s="38"/>
       <c r="M54" s="38"/>
       <c r="N54" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="O54" s="21" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="P54" s="21" t="s">
         <v>309</v>
       </c>
       <c r="Q54" s="21" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="R54" s="66" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="S54" s="46" t="s">
         <v>36</v>
@@ -19940,19 +19958,19 @@
       <c r="L55" s="38"/>
       <c r="M55" s="38"/>
       <c r="N55" t="s">
-        <v>398</v>
+        <v>310</v>
       </c>
       <c r="O55" s="21" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="P55" s="21" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="Q55" s="21" t="s">
-        <v>267</v>
+        <v>331</v>
       </c>
       <c r="R55" s="66" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="S55" s="46" t="s">
         <v>36</v>
@@ -19965,19 +19983,19 @@
       <c r="L56" s="38"/>
       <c r="M56" s="38"/>
       <c r="N56" t="s">
-        <v>399</v>
+        <v>312</v>
       </c>
       <c r="O56" s="21" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="P56" s="21" t="s">
-        <v>267</v>
+        <v>309</v>
       </c>
       <c r="Q56" s="21" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="R56" s="66" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="S56" s="46" t="s">
         <v>36</v>
@@ -19990,19 +20008,19 @@
       <c r="L57" s="38"/>
       <c r="M57" s="38"/>
       <c r="N57" t="s">
-        <v>313</v>
+        <v>398</v>
       </c>
       <c r="O57" s="21" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="P57" s="21" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="Q57" s="21" t="s">
-        <v>41</v>
+        <v>267</v>
       </c>
       <c r="R57" s="66" t="s">
-        <v>314</v>
+        <v>400</v>
       </c>
       <c r="S57" s="46" t="s">
         <v>36</v>
@@ -20015,19 +20033,19 @@
       <c r="L58" s="38"/>
       <c r="M58" s="38"/>
       <c r="N58" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="O58" s="21" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="P58" s="21" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="Q58" s="21" t="s">
-        <v>267</v>
+        <v>401</v>
       </c>
       <c r="R58" s="66" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="S58" s="46" t="s">
         <v>36</v>
@@ -20040,19 +20058,19 @@
       <c r="L59" s="38"/>
       <c r="M59" s="38"/>
       <c r="N59" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O59" s="21" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="P59" s="21" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="Q59" s="21" t="s">
-        <v>267</v>
+        <v>41</v>
       </c>
       <c r="R59" s="66" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="S59" s="46" t="s">
         <v>36</v>
@@ -20065,19 +20083,19 @@
       <c r="L60" s="38"/>
       <c r="M60" s="38"/>
       <c r="N60" t="s">
-        <v>317</v>
+        <v>405</v>
       </c>
       <c r="O60" s="21" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="P60" s="21" t="s">
-        <v>318</v>
+        <v>266</v>
       </c>
       <c r="Q60" s="21" t="s">
-        <v>410</v>
+        <v>267</v>
       </c>
       <c r="R60" s="66" t="s">
-        <v>319</v>
+        <v>406</v>
       </c>
       <c r="S60" s="46" t="s">
         <v>36</v>
@@ -20090,173 +20108,171 @@
       <c r="L61" s="38"/>
       <c r="M61" s="38"/>
       <c r="N61" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="O61" s="21" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="P61" s="21" t="s">
-        <v>309</v>
+        <v>266</v>
       </c>
       <c r="Q61" s="21" t="s">
-        <v>412</v>
+        <v>267</v>
       </c>
       <c r="R61" s="66" t="s">
-        <v>413</v>
+        <v>316</v>
       </c>
       <c r="S61" s="46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="62" spans="4:19">
-      <c r="D62" s="8"/>
       <c r="I62" s="8"/>
       <c r="J62" s="38"/>
       <c r="K62" s="38"/>
       <c r="L62" s="38"/>
       <c r="M62" s="38"/>
       <c r="N62" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="O62" s="21" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="P62" s="21" t="s">
-        <v>45</v>
+        <v>318</v>
       </c>
       <c r="Q62" s="21" t="s">
-        <v>299</v>
+        <v>410</v>
       </c>
       <c r="R62" s="66" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="S62" s="46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="63" spans="4:19">
-      <c r="D63" s="8"/>
       <c r="I63" s="8"/>
       <c r="J63" s="38"/>
       <c r="K63" s="38"/>
       <c r="L63" s="38"/>
       <c r="M63" s="38"/>
       <c r="N63" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="O63" s="21" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="P63" s="21" t="s">
-        <v>42</v>
+        <v>309</v>
       </c>
       <c r="Q63" s="21" t="s">
-        <v>267</v>
+        <v>412</v>
       </c>
       <c r="R63" s="66" t="s">
-        <v>324</v>
+        <v>413</v>
       </c>
       <c r="S63" s="46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="64" spans="4:19">
+      <c r="D64" s="8"/>
       <c r="I64" s="8"/>
       <c r="J64" s="38"/>
       <c r="K64" s="38"/>
       <c r="L64" s="38"/>
       <c r="M64" s="38"/>
       <c r="N64" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="O64" s="21" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="P64" s="21" t="s">
-        <v>309</v>
+        <v>45</v>
       </c>
       <c r="Q64" s="21" t="s">
         <v>299</v>
       </c>
       <c r="R64" s="66" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="S64" s="46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="65" spans="4:19">
+      <c r="D65" s="8"/>
       <c r="I65" s="8"/>
       <c r="J65" s="38"/>
       <c r="K65" s="38"/>
       <c r="L65" s="38"/>
       <c r="M65" s="38"/>
       <c r="N65" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="O65" s="21" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="P65" s="21" t="s">
-        <v>311</v>
+        <v>42</v>
       </c>
       <c r="Q65" s="21" t="s">
-        <v>328</v>
+        <v>267</v>
       </c>
       <c r="R65" s="66" t="s">
-        <v>420</v>
+        <v>324</v>
       </c>
       <c r="S65" s="46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="66" spans="4:19">
-      <c r="D66" s="8"/>
       <c r="I66" s="8"/>
       <c r="J66" s="38"/>
       <c r="K66" s="38"/>
       <c r="L66" s="38"/>
       <c r="M66" s="38"/>
       <c r="N66" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="O66" s="21" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P66" s="21" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="Q66" s="21" t="s">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="R66" s="66" t="s">
-        <v>421</v>
+        <v>326</v>
       </c>
       <c r="S66" s="46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="67" spans="4:19">
-      <c r="D67" s="8"/>
       <c r="I67" s="8"/>
       <c r="J67" s="38"/>
       <c r="K67" s="38"/>
       <c r="L67" s="38"/>
       <c r="M67" s="38"/>
       <c r="N67" t="s">
-        <v>422</v>
+        <v>327</v>
       </c>
       <c r="O67" s="21" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="P67" s="21" t="s">
-        <v>276</v>
+        <v>311</v>
       </c>
       <c r="Q67" s="21" t="s">
-        <v>423</v>
+        <v>328</v>
       </c>
       <c r="R67" s="66" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="S67" s="46" t="s">
         <v>36</v>
@@ -20270,19 +20286,19 @@
       <c r="L68" s="38"/>
       <c r="M68" s="38"/>
       <c r="N68" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="O68" s="21" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="P68" s="21" t="s">
-        <v>41</v>
+        <v>330</v>
       </c>
       <c r="Q68" s="21" t="s">
-        <v>426</v>
+        <v>331</v>
       </c>
       <c r="R68" s="66" t="s">
-        <v>457</v>
+        <v>421</v>
       </c>
       <c r="S68" s="46" t="s">
         <v>36</v>
@@ -20296,19 +20312,19 @@
       <c r="L69" s="38"/>
       <c r="M69" s="38"/>
       <c r="N69" t="s">
-        <v>333</v>
+        <v>422</v>
       </c>
       <c r="O69" s="21" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="P69" s="21" t="s">
-        <v>131</v>
+        <v>276</v>
       </c>
       <c r="Q69" s="21" t="s">
-        <v>309</v>
+        <v>423</v>
       </c>
       <c r="R69" s="66" t="s">
-        <v>334</v>
+        <v>424</v>
       </c>
       <c r="S69" s="46" t="s">
         <v>36</v>
@@ -20322,69 +20338,71 @@
       <c r="L70" s="38"/>
       <c r="M70" s="38"/>
       <c r="N70" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="O70" s="21" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="P70" s="21" t="s">
-        <v>266</v>
+        <v>41</v>
       </c>
       <c r="Q70" s="21" t="s">
-        <v>299</v>
+        <v>426</v>
       </c>
       <c r="R70" s="66" t="s">
-        <v>336</v>
+        <v>457</v>
       </c>
       <c r="S70" s="46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="71" spans="4:19">
+      <c r="D71" s="8"/>
       <c r="I71" s="8"/>
       <c r="J71" s="38"/>
       <c r="K71" s="38"/>
       <c r="L71" s="38"/>
       <c r="M71" s="38"/>
       <c r="N71" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="O71" s="21" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="P71" s="21" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
       <c r="Q71" s="21" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="R71" s="66" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="S71" s="46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="72" spans="4:19">
+      <c r="D72" s="8"/>
       <c r="I72" s="8"/>
       <c r="J72" s="38"/>
       <c r="K72" s="38"/>
       <c r="L72" s="38"/>
       <c r="M72" s="38"/>
       <c r="N72" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="O72" s="21" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="P72" s="21" t="s">
-        <v>311</v>
+        <v>266</v>
       </c>
       <c r="Q72" s="21" t="s">
-        <v>328</v>
+        <v>299</v>
       </c>
       <c r="R72" s="66" t="s">
-        <v>430</v>
+        <v>336</v>
       </c>
       <c r="S72" s="46" t="s">
         <v>36</v>
@@ -20397,19 +20415,19 @@
       <c r="L73" s="38"/>
       <c r="M73" s="38"/>
       <c r="N73" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="O73" s="21" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="P73" s="21" t="s">
-        <v>311</v>
+        <v>41</v>
       </c>
       <c r="Q73" s="21" t="s">
-        <v>267</v>
+        <v>299</v>
       </c>
       <c r="R73" s="66" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="S73" s="46" t="s">
         <v>36</v>
@@ -20422,19 +20440,19 @@
       <c r="L74" s="38"/>
       <c r="M74" s="38"/>
       <c r="N74" t="s">
-        <v>433</v>
+        <v>339</v>
       </c>
       <c r="O74" s="21" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="P74" s="21" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="Q74" s="21" t="s">
-        <v>267</v>
+        <v>328</v>
       </c>
       <c r="R74" s="66" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="S74" s="46" t="s">
         <v>36</v>
@@ -20447,19 +20465,19 @@
       <c r="L75" s="38"/>
       <c r="M75" s="38"/>
       <c r="N75" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="O75" s="21" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="P75" s="21" t="s">
-        <v>265</v>
+        <v>311</v>
       </c>
       <c r="Q75" s="21" t="s">
-        <v>436</v>
+        <v>267</v>
       </c>
       <c r="R75" s="66" t="s">
-        <v>437</v>
+        <v>341</v>
       </c>
       <c r="S75" s="46" t="s">
         <v>36</v>
@@ -20472,19 +20490,19 @@
       <c r="L76" s="38"/>
       <c r="M76" s="38"/>
       <c r="N76" t="s">
-        <v>343</v>
+        <v>433</v>
       </c>
       <c r="O76" s="21" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="P76" s="21" t="s">
-        <v>265</v>
+        <v>299</v>
       </c>
       <c r="Q76" s="21" t="s">
-        <v>41</v>
+        <v>267</v>
       </c>
       <c r="R76" s="66" t="s">
-        <v>344</v>
+        <v>434</v>
       </c>
       <c r="S76" s="46" t="s">
         <v>36</v>
@@ -20497,19 +20515,19 @@
       <c r="L77" s="38"/>
       <c r="M77" s="38"/>
       <c r="N77" t="s">
-        <v>440</v>
+        <v>342</v>
       </c>
       <c r="O77" s="21" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="P77" s="21" t="s">
-        <v>41</v>
+        <v>265</v>
       </c>
       <c r="Q77" s="21" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="R77" s="66" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="S77" s="46" t="s">
         <v>36</v>
@@ -20522,19 +20540,19 @@
       <c r="L78" s="38"/>
       <c r="M78" s="38"/>
       <c r="N78" t="s">
-        <v>444</v>
+        <v>343</v>
       </c>
       <c r="O78" s="21" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="P78" s="21" t="s">
-        <v>46</v>
+        <v>265</v>
       </c>
       <c r="Q78" s="21" t="s">
-        <v>265</v>
+        <v>41</v>
       </c>
       <c r="R78" s="66" t="s">
-        <v>445</v>
+        <v>344</v>
       </c>
       <c r="S78" s="46" t="s">
         <v>36</v>
@@ -20547,19 +20565,19 @@
       <c r="L79" s="38"/>
       <c r="M79" s="38"/>
       <c r="N79" t="s">
-        <v>345</v>
+        <v>440</v>
       </c>
       <c r="O79" s="21" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="P79" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q79" s="21" t="s">
-        <v>346</v>
+        <v>441</v>
       </c>
       <c r="R79" s="66" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="S79" s="46" t="s">
         <v>36</v>
@@ -20572,19 +20590,19 @@
       <c r="L80" s="38"/>
       <c r="M80" s="38"/>
       <c r="N80" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="O80" s="21" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="P80" s="21" t="s">
-        <v>309</v>
+        <v>46</v>
       </c>
       <c r="Q80" s="21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="R80" s="66" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="S80" s="46" t="s">
         <v>36</v>
@@ -20597,19 +20615,19 @@
       <c r="L81" s="38"/>
       <c r="M81" s="38"/>
       <c r="N81" t="s">
-        <v>451</v>
+        <v>345</v>
       </c>
       <c r="O81" s="21" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="P81" s="21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q81" s="21" t="s">
-        <v>131</v>
+        <v>346</v>
       </c>
       <c r="R81" s="66" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="S81" s="46" t="s">
         <v>36</v>
@@ -20622,19 +20640,19 @@
       <c r="L82" s="38"/>
       <c r="M82" s="38"/>
       <c r="N82" t="s">
-        <v>347</v>
+        <v>448</v>
       </c>
       <c r="O82" s="21" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="P82" s="21" t="s">
-        <v>265</v>
+        <v>309</v>
       </c>
       <c r="Q82" s="21" t="s">
-        <v>348</v>
+        <v>267</v>
       </c>
       <c r="R82" s="66" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="S82" s="46" t="s">
         <v>36</v>
@@ -20647,19 +20665,19 @@
       <c r="L83" s="38"/>
       <c r="M83" s="38"/>
       <c r="N83" t="s">
-        <v>349</v>
+        <v>451</v>
       </c>
       <c r="O83" s="21" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="P83" s="21" t="s">
-        <v>294</v>
+        <v>45</v>
       </c>
       <c r="Q83" s="21" t="s">
-        <v>267</v>
+        <v>131</v>
       </c>
       <c r="R83" s="66" t="s">
-        <v>350</v>
+        <v>452</v>
       </c>
       <c r="S83" s="46" t="s">
         <v>36</v>
@@ -20672,19 +20690,19 @@
       <c r="L84" s="38"/>
       <c r="M84" s="38"/>
       <c r="N84" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="O84" s="21" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="P84" s="21" t="s">
-        <v>42</v>
+        <v>265</v>
       </c>
       <c r="Q84" s="21" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="R84" s="66" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="S84" s="46" t="s">
         <v>36</v>
@@ -20697,77 +20715,73 @@
       <c r="L85" s="38"/>
       <c r="M85" s="38"/>
       <c r="N85" t="s">
-        <v>461</v>
+        <v>349</v>
       </c>
       <c r="O85" s="21" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="P85" s="21" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="Q85" s="21" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="R85" s="66" t="s">
-        <v>462</v>
+        <v>350</v>
       </c>
       <c r="S85" s="46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="86" spans="4:20">
-      <c r="D86" s="8"/>
       <c r="I86" s="8"/>
       <c r="J86" s="38"/>
       <c r="K86" s="38"/>
       <c r="L86" s="38"/>
       <c r="M86" s="38"/>
       <c r="N86" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="O86" s="21" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="P86" s="21" t="s">
-        <v>265</v>
+        <v>42</v>
       </c>
       <c r="Q86" s="21" t="s">
-        <v>41</v>
+        <v>352</v>
       </c>
       <c r="R86" s="66" t="s">
-        <v>354</v>
+        <v>460</v>
       </c>
       <c r="S86" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="T86" s="31"/>
     </row>
     <row r="87" spans="4:20">
-      <c r="D87" s="8"/>
       <c r="I87" s="8"/>
       <c r="J87" s="38"/>
       <c r="K87" s="38"/>
       <c r="L87" s="38"/>
       <c r="M87" s="38"/>
       <c r="N87" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="O87" s="21" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="P87" s="21" t="s">
         <v>311</v>
       </c>
       <c r="Q87" s="21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="R87" s="66" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="S87" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="T87" s="31"/>
     </row>
     <row r="88" spans="4:20">
       <c r="D88" s="8"/>
@@ -20777,19 +20791,19 @@
       <c r="L88" s="38"/>
       <c r="M88" s="38"/>
       <c r="N88" t="s">
-        <v>466</v>
+        <v>353</v>
       </c>
       <c r="O88" s="21" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="P88" s="21" t="s">
-        <v>42</v>
+        <v>265</v>
       </c>
       <c r="Q88" s="21" t="s">
-        <v>267</v>
+        <v>41</v>
       </c>
       <c r="R88" s="66" t="s">
-        <v>472</v>
+        <v>354</v>
       </c>
       <c r="S88" s="46" t="s">
         <v>36</v>
@@ -20804,19 +20818,19 @@
       <c r="L89" s="38"/>
       <c r="M89" s="38"/>
       <c r="N89" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="O89" s="21" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="P89" s="21" t="s">
-        <v>41</v>
+        <v>311</v>
       </c>
       <c r="Q89" s="21" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="R89" s="66" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="S89" s="46" t="s">
         <v>36</v>
@@ -20831,10 +20845,10 @@
       <c r="L90" s="38"/>
       <c r="M90" s="38"/>
       <c r="N90" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="O90" s="21" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="P90" s="21" t="s">
         <v>42</v>
@@ -20843,7 +20857,7 @@
         <v>267</v>
       </c>
       <c r="R90" s="66" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="S90" s="46" t="s">
         <v>36</v>
@@ -20858,48 +20872,51 @@
       <c r="L91" s="38"/>
       <c r="M91" s="38"/>
       <c r="N91" t="s">
-        <v>355</v>
+        <v>467</v>
       </c>
       <c r="O91" s="21" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="P91" s="21" t="s">
-        <v>311</v>
+        <v>41</v>
       </c>
       <c r="Q91" s="21" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="R91" s="66" t="s">
-        <v>356</v>
+        <v>474</v>
       </c>
       <c r="S91" s="46" t="s">
         <v>36</v>
       </c>
+      <c r="T91" s="31"/>
     </row>
     <row r="92" spans="4:20">
+      <c r="D92" s="8"/>
       <c r="I92" s="8"/>
       <c r="J92" s="38"/>
       <c r="K92" s="38"/>
       <c r="L92" s="38"/>
       <c r="M92" s="38"/>
       <c r="N92" t="s">
-        <v>357</v>
+        <v>468</v>
       </c>
       <c r="O92" s="21" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="P92" s="21" t="s">
-        <v>358</v>
+        <v>42</v>
       </c>
       <c r="Q92" s="21" t="s">
-        <v>478</v>
+        <v>267</v>
       </c>
       <c r="R92" s="66" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
       <c r="S92" s="46" t="s">
         <v>36</v>
       </c>
+      <c r="T92" s="31"/>
     </row>
     <row r="93" spans="4:20">
       <c r="D93" s="8"/>
@@ -20909,106 +20926,114 @@
       <c r="L93" s="38"/>
       <c r="M93" s="38"/>
       <c r="N93" t="s">
-        <v>480</v>
+        <v>355</v>
       </c>
       <c r="O93" s="21" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="P93" s="21" t="s">
-        <v>265</v>
+        <v>311</v>
       </c>
       <c r="Q93" s="21" t="s">
-        <v>436</v>
+        <v>267</v>
       </c>
       <c r="R93" s="66" t="s">
-        <v>482</v>
+        <v>356</v>
       </c>
       <c r="S93" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="T93" s="31"/>
     </row>
     <row r="94" spans="4:20">
       <c r="I94" s="8"/>
-      <c r="J94" s="35" t="s">
-        <v>553</v>
-      </c>
-      <c r="K94" s="36">
-        <v>2715342</v>
-      </c>
-      <c r="L94" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="M94" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="R94" t="s">
-        <v>89</v>
-      </c>
-      <c r="S94" s="31" t="s">
-        <v>49</v>
+      <c r="J94" s="38"/>
+      <c r="K94" s="38"/>
+      <c r="L94" s="38"/>
+      <c r="M94" s="38"/>
+      <c r="N94" t="s">
+        <v>357</v>
+      </c>
+      <c r="O94" s="21" t="s">
+        <v>479</v>
+      </c>
+      <c r="P94" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="Q94" s="21" t="s">
+        <v>478</v>
+      </c>
+      <c r="R94" s="66" t="s">
+        <v>359</v>
+      </c>
+      <c r="S94" s="46" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="95" spans="4:20">
       <c r="D95" s="8"/>
       <c r="I95" s="8"/>
-      <c r="J95" s="35" t="s">
-        <v>554</v>
-      </c>
-      <c r="K95" s="36">
-        <v>2715344</v>
-      </c>
-      <c r="L95" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="M95" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="R95" t="s">
-        <v>90</v>
-      </c>
-      <c r="S95" s="31" t="s">
-        <v>49</v>
-      </c>
+      <c r="J95" s="38"/>
+      <c r="K95" s="38"/>
+      <c r="L95" s="38"/>
+      <c r="M95" s="38"/>
+      <c r="N95" t="s">
+        <v>480</v>
+      </c>
+      <c r="O95" s="21" t="s">
+        <v>481</v>
+      </c>
+      <c r="P95" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q95" s="21" t="s">
+        <v>436</v>
+      </c>
+      <c r="R95" s="66" t="s">
+        <v>482</v>
+      </c>
+      <c r="S95" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="T95" s="31"/>
     </row>
     <row r="96" spans="4:20">
-      <c r="D96" s="8"/>
-      <c r="I96" s="10"/>
-      <c r="J96" s="37" t="s">
-        <v>555</v>
+      <c r="I96" s="8"/>
+      <c r="J96" s="35" t="s">
+        <v>551</v>
       </c>
       <c r="K96" s="36">
-        <v>2715346</v>
+        <v>2715342</v>
       </c>
       <c r="L96" s="36" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="M96" s="36" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="R96" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S96" s="31" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="97" spans="1:32">
+      <c r="D97" s="8"/>
       <c r="I97" s="8"/>
       <c r="J97" s="35" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="K97" s="36">
-        <v>2715369</v>
+        <v>2715344</v>
       </c>
       <c r="L97" s="36" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="M97" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="R97" s="22" t="s">
-        <v>93</v>
+      <c r="R97" t="s">
+        <v>90</v>
       </c>
       <c r="S97" s="31" t="s">
         <v>49</v>
@@ -21016,67 +21041,102 @@
     </row>
     <row r="98" spans="1:32">
       <c r="D98" s="8"/>
-      <c r="I98" s="8"/>
-      <c r="S98" s="31"/>
+      <c r="I98" s="10"/>
+      <c r="J98" s="37" t="s">
+        <v>553</v>
+      </c>
+      <c r="K98" s="36">
+        <v>2715346</v>
+      </c>
+      <c r="L98" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="M98" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="R98" t="s">
+        <v>91</v>
+      </c>
+      <c r="S98" s="31" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="99" spans="1:32">
       <c r="I99" s="8"/>
-      <c r="R99" s="5"/>
-      <c r="S99" s="31"/>
-      <c r="AD99" s="6"/>
-      <c r="AE99" s="7"/>
-      <c r="AF99" s="5"/>
+      <c r="J99" s="35" t="s">
+        <v>554</v>
+      </c>
+      <c r="K99" s="36">
+        <v>2715369</v>
+      </c>
+      <c r="L99" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="M99" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="R99" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="S99" s="31" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="100" spans="1:32">
-      <c r="A100" s="16"/>
-      <c r="B100" s="17"/>
-      <c r="C100" s="5"/>
-      <c r="D100" s="18"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="5"/>
-      <c r="G100" s="5"/>
-      <c r="H100" s="5"/>
-      <c r="I100" s="20"/>
-      <c r="J100" s="30"/>
-      <c r="K100" s="27"/>
-      <c r="L100" s="27"/>
-      <c r="M100" s="27"/>
-      <c r="N100" s="5"/>
-      <c r="O100" s="5"/>
-      <c r="P100" s="5"/>
-      <c r="Q100" s="5"/>
-      <c r="R100" s="5"/>
-      <c r="S100" s="32"/>
-      <c r="T100" s="5"/>
-      <c r="U100" s="5"/>
-      <c r="V100" s="5"/>
-      <c r="W100" s="5"/>
-      <c r="X100" s="5"/>
-      <c r="Y100" s="5"/>
-      <c r="Z100" s="5"/>
-      <c r="AA100" s="5"/>
-      <c r="AB100" s="5"/>
-      <c r="AC100" s="5"/>
-      <c r="AD100" s="6"/>
-      <c r="AE100" s="7"/>
-      <c r="AF100" s="5"/>
+      <c r="D100" s="8"/>
+      <c r="I100" s="8"/>
+      <c r="S100" s="31"/>
     </row>
     <row r="101" spans="1:32">
       <c r="I101" s="8"/>
       <c r="R101" s="5"/>
       <c r="S101" s="31"/>
+      <c r="AD101" s="6"/>
+      <c r="AE101" s="7"/>
+      <c r="AF101" s="5"/>
     </row>
     <row r="102" spans="1:32">
-      <c r="I102" s="8"/>
+      <c r="A102" s="16"/>
+      <c r="B102" s="17"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+      <c r="I102" s="20"/>
+      <c r="J102" s="30"/>
+      <c r="K102" s="27"/>
+      <c r="L102" s="27"/>
+      <c r="M102" s="27"/>
+      <c r="N102" s="5"/>
+      <c r="O102" s="5"/>
+      <c r="P102" s="5"/>
+      <c r="Q102" s="5"/>
       <c r="R102" s="5"/>
-      <c r="S102" s="31"/>
+      <c r="S102" s="32"/>
+      <c r="T102" s="5"/>
+      <c r="U102" s="5"/>
+      <c r="V102" s="5"/>
+      <c r="W102" s="5"/>
+      <c r="X102" s="5"/>
+      <c r="Y102" s="5"/>
+      <c r="Z102" s="5"/>
+      <c r="AA102" s="5"/>
+      <c r="AB102" s="5"/>
+      <c r="AC102" s="5"/>
+      <c r="AD102" s="6"/>
+      <c r="AE102" s="7"/>
+      <c r="AF102" s="5"/>
     </row>
     <row r="103" spans="1:32">
       <c r="I103" s="8"/>
+      <c r="R103" s="5"/>
       <c r="S103" s="31"/>
     </row>
     <row r="104" spans="1:32">
       <c r="I104" s="8"/>
+      <c r="R104" s="5"/>
       <c r="S104" s="31"/>
     </row>
     <row r="105" spans="1:32">
@@ -21084,18 +21144,18 @@
       <c r="S105" s="31"/>
     </row>
     <row r="106" spans="1:32">
-      <c r="D106" s="8"/>
       <c r="I106" s="8"/>
       <c r="S106" s="31"/>
-      <c r="T106" s="31"/>
     </row>
     <row r="107" spans="1:32">
       <c r="I107" s="8"/>
       <c r="S107" s="31"/>
     </row>
     <row r="108" spans="1:32">
+      <c r="D108" s="8"/>
       <c r="I108" s="8"/>
       <c r="S108" s="31"/>
+      <c r="T108" s="31"/>
     </row>
     <row r="109" spans="1:32">
       <c r="I109" s="8"/>
@@ -21130,26 +21190,26 @@
       <c r="S116" s="31"/>
     </row>
     <row r="117" spans="4:19">
-      <c r="D117" s="8"/>
-      <c r="I117" s="10"/>
-      <c r="J117" s="29"/>
-      <c r="S117" s="32"/>
+      <c r="I117" s="8"/>
+      <c r="S117" s="31"/>
     </row>
     <row r="118" spans="4:19">
       <c r="I118" s="8"/>
-      <c r="R118" s="22"/>
-      <c r="S118" s="33"/>
+      <c r="S118" s="31"/>
     </row>
     <row r="119" spans="4:19">
       <c r="D119" s="8"/>
-      <c r="I119" s="8"/>
-      <c r="S119" s="31"/>
+      <c r="I119" s="10"/>
+      <c r="J119" s="29"/>
+      <c r="S119" s="32"/>
     </row>
     <row r="120" spans="4:19">
       <c r="I120" s="8"/>
-      <c r="S120" s="31"/>
+      <c r="R120" s="22"/>
+      <c r="S120" s="33"/>
     </row>
     <row r="121" spans="4:19">
+      <c r="D121" s="8"/>
       <c r="I121" s="8"/>
       <c r="S121" s="31"/>
     </row>
@@ -21182,12 +21242,10 @@
       <c r="S128" s="31"/>
     </row>
     <row r="129" spans="4:19">
-      <c r="D129" s="8"/>
       <c r="I129" s="8"/>
       <c r="S129" s="31"/>
     </row>
     <row r="130" spans="4:19">
-      <c r="D130" s="8"/>
       <c r="I130" s="8"/>
       <c r="S130" s="31"/>
     </row>
@@ -21202,76 +21260,76 @@
       <c r="S132" s="31"/>
     </row>
     <row r="133" spans="4:19">
+      <c r="D133" s="8"/>
       <c r="I133" s="8"/>
-      <c r="S133" s="34"/>
+      <c r="S133" s="31"/>
     </row>
     <row r="134" spans="4:19">
+      <c r="D134" s="8"/>
       <c r="I134" s="8"/>
-      <c r="S134" s="34"/>
+      <c r="S134" s="31"/>
     </row>
     <row r="135" spans="4:19">
       <c r="I135" s="8"/>
-      <c r="S135" s="32"/>
+      <c r="S135" s="34"/>
     </row>
     <row r="136" spans="4:19">
       <c r="I136" s="8"/>
-      <c r="S136" s="31"/>
+      <c r="S136" s="34"/>
     </row>
     <row r="137" spans="4:19">
       <c r="I137" s="8"/>
-      <c r="S137" s="31"/>
+      <c r="S137" s="32"/>
     </row>
     <row r="138" spans="4:19">
       <c r="I138" s="8"/>
-      <c r="S138" s="32"/>
+      <c r="S138" s="31"/>
     </row>
     <row r="139" spans="4:19">
       <c r="I139" s="8"/>
-      <c r="S139" s="32"/>
+      <c r="S139" s="31"/>
     </row>
     <row r="140" spans="4:19">
       <c r="I140" s="8"/>
       <c r="S140" s="32"/>
     </row>
     <row r="141" spans="4:19">
-      <c r="R141" s="22"/>
-      <c r="S141" s="33"/>
+      <c r="I141" s="8"/>
+      <c r="S141" s="32"/>
     </row>
     <row r="142" spans="4:19">
-      <c r="R142" s="22"/>
-      <c r="S142" s="33"/>
+      <c r="I142" s="8"/>
+      <c r="S142" s="32"/>
     </row>
     <row r="143" spans="4:19">
-      <c r="D143" s="8"/>
-      <c r="I143" s="8"/>
-      <c r="S143" s="34"/>
+      <c r="R143" s="22"/>
+      <c r="S143" s="33"/>
     </row>
     <row r="144" spans="4:19">
-      <c r="D144" s="8"/>
-      <c r="I144" s="8"/>
-      <c r="S144" s="34"/>
+      <c r="R144" s="22"/>
+      <c r="S144" s="33"/>
     </row>
     <row r="145" spans="4:19">
       <c r="D145" s="8"/>
-      <c r="I145" s="10"/>
-      <c r="J145" s="29"/>
-      <c r="S145" s="32"/>
+      <c r="I145" s="8"/>
+      <c r="S145" s="34"/>
     </row>
     <row r="146" spans="4:19">
       <c r="D146" s="8"/>
-      <c r="I146" s="10"/>
-      <c r="J146" s="29"/>
-      <c r="S146" s="32"/>
+      <c r="I146" s="8"/>
+      <c r="S146" s="34"/>
     </row>
     <row r="147" spans="4:19">
       <c r="D147" s="8"/>
-      <c r="I147" s="8"/>
-      <c r="S147" s="31"/>
+      <c r="I147" s="10"/>
+      <c r="J147" s="29"/>
+      <c r="S147" s="32"/>
     </row>
     <row r="148" spans="4:19">
       <c r="D148" s="8"/>
-      <c r="I148" s="8"/>
-      <c r="S148" s="31"/>
+      <c r="I148" s="10"/>
+      <c r="J148" s="29"/>
+      <c r="S148" s="32"/>
     </row>
     <row r="149" spans="4:19">
       <c r="D149" s="8"/>
@@ -21284,10 +21342,12 @@
       <c r="S150" s="31"/>
     </row>
     <row r="151" spans="4:19">
+      <c r="D151" s="8"/>
       <c r="I151" s="8"/>
       <c r="S151" s="31"/>
     </row>
     <row r="152" spans="4:19">
+      <c r="D152" s="8"/>
       <c r="I152" s="8"/>
       <c r="S152" s="31"/>
     </row>
@@ -21305,12 +21365,10 @@
     </row>
     <row r="156" spans="4:19">
       <c r="I156" s="8"/>
-      <c r="R156" s="11"/>
       <c r="S156" s="31"/>
     </row>
     <row r="157" spans="4:19">
       <c r="I157" s="8"/>
-      <c r="R157" s="11"/>
       <c r="S157" s="31"/>
     </row>
     <row r="158" spans="4:19">
@@ -21329,33 +21387,33 @@
       <c r="S160" s="31"/>
     </row>
     <row r="161" spans="4:20">
-      <c r="D161" s="8"/>
       <c r="I161" s="8"/>
+      <c r="R161" s="11"/>
       <c r="S161" s="31"/>
     </row>
     <row r="162" spans="4:20">
-      <c r="D162" s="8"/>
       <c r="I162" s="8"/>
+      <c r="R162" s="11"/>
       <c r="S162" s="31"/>
     </row>
     <row r="163" spans="4:20">
+      <c r="D163" s="8"/>
       <c r="I163" s="8"/>
-      <c r="R163" s="12"/>
       <c r="S163" s="31"/>
     </row>
     <row r="164" spans="4:20">
+      <c r="D164" s="8"/>
       <c r="I164" s="8"/>
-      <c r="R164" s="12"/>
       <c r="S164" s="31"/>
     </row>
     <row r="165" spans="4:20">
-      <c r="D165" s="8"/>
       <c r="I165" s="8"/>
+      <c r="R165" s="12"/>
       <c r="S165" s="31"/>
     </row>
     <row r="166" spans="4:20">
-      <c r="D166" s="8"/>
       <c r="I166" s="8"/>
+      <c r="R166" s="12"/>
       <c r="S166" s="31"/>
     </row>
     <row r="167" spans="4:20">
@@ -21377,7 +21435,6 @@
       <c r="D170" s="8"/>
       <c r="I170" s="8"/>
       <c r="S170" s="31"/>
-      <c r="T170" s="14"/>
     </row>
     <row r="171" spans="4:20">
       <c r="D171" s="8"/>
@@ -21387,15 +21444,18 @@
     <row r="172" spans="4:20">
       <c r="D172" s="8"/>
       <c r="I172" s="8"/>
-      <c r="R172" s="21"/>
       <c r="S172" s="31"/>
+      <c r="T172" s="14"/>
     </row>
     <row r="173" spans="4:20">
+      <c r="D173" s="8"/>
       <c r="I173" s="8"/>
       <c r="S173" s="31"/>
     </row>
     <row r="174" spans="4:20">
+      <c r="D174" s="8"/>
       <c r="I174" s="8"/>
+      <c r="R174" s="21"/>
       <c r="S174" s="31"/>
     </row>
     <row r="175" spans="4:20">
@@ -21432,83 +21492,85 @@
     </row>
     <row r="183" spans="1:32">
       <c r="I183" s="8"/>
-      <c r="R183" s="22"/>
       <c r="S183" s="31"/>
     </row>
     <row r="184" spans="1:32">
-      <c r="D184" s="8"/>
       <c r="I184" s="8"/>
       <c r="S184" s="31"/>
     </row>
-    <row r="185" spans="1:32" s="13" customFormat="1">
-      <c r="A185"/>
-      <c r="B185"/>
-      <c r="C185"/>
-      <c r="D185"/>
-      <c r="E185"/>
-      <c r="F185"/>
-      <c r="G185"/>
-      <c r="H185"/>
-      <c r="I185"/>
-      <c r="J185" s="28"/>
-      <c r="K185" s="28"/>
-      <c r="L185" s="28"/>
-      <c r="M185" s="28"/>
-      <c r="N185"/>
-      <c r="O185"/>
-      <c r="P185"/>
-      <c r="Q185"/>
-      <c r="R185"/>
+    <row r="185" spans="1:32">
+      <c r="I185" s="8"/>
+      <c r="R185" s="22"/>
       <c r="S185" s="31"/>
-      <c r="T185"/>
-      <c r="U185"/>
-      <c r="V185"/>
-      <c r="W185"/>
-      <c r="X185"/>
-      <c r="Y185"/>
-      <c r="Z185"/>
-      <c r="AA185"/>
-      <c r="AB185"/>
-      <c r="AC185"/>
-      <c r="AD185"/>
-      <c r="AE185"/>
-      <c r="AF185"/>
     </row>
     <row r="186" spans="1:32">
+      <c r="D186" s="8"/>
+      <c r="I186" s="8"/>
       <c r="S186" s="31"/>
     </row>
-    <row r="187" spans="1:32">
-      <c r="I187" s="8"/>
-      <c r="R187" s="21"/>
+    <row r="187" spans="1:32" s="13" customFormat="1">
+      <c r="A187"/>
+      <c r="B187"/>
+      <c r="C187"/>
+      <c r="D187"/>
+      <c r="E187"/>
+      <c r="F187"/>
+      <c r="G187"/>
+      <c r="H187"/>
+      <c r="I187"/>
+      <c r="J187" s="28"/>
+      <c r="K187" s="28"/>
+      <c r="L187" s="28"/>
+      <c r="M187" s="28"/>
+      <c r="N187"/>
+      <c r="O187"/>
+      <c r="P187"/>
+      <c r="Q187"/>
+      <c r="R187"/>
       <c r="S187" s="31"/>
+      <c r="T187"/>
+      <c r="U187"/>
+      <c r="V187"/>
+      <c r="W187"/>
+      <c r="X187"/>
+      <c r="Y187"/>
+      <c r="Z187"/>
+      <c r="AA187"/>
+      <c r="AB187"/>
+      <c r="AC187"/>
+      <c r="AD187"/>
+      <c r="AE187"/>
+      <c r="AF187"/>
     </row>
     <row r="188" spans="1:32">
-      <c r="D188" s="8"/>
       <c r="S188" s="31"/>
     </row>
     <row r="189" spans="1:32">
+      <c r="I189" s="8"/>
+      <c r="R189" s="21"/>
       <c r="S189" s="31"/>
     </row>
     <row r="190" spans="1:32">
+      <c r="D190" s="8"/>
       <c r="S190" s="31"/>
     </row>
     <row r="191" spans="1:32">
-      <c r="D191" s="8"/>
-      <c r="I191" s="8"/>
       <c r="S191" s="31"/>
     </row>
     <row r="192" spans="1:32">
-      <c r="I192" s="8"/>
       <c r="S192" s="31"/>
     </row>
     <row r="193" spans="4:19">
       <c r="D193" s="8"/>
+      <c r="I193" s="8"/>
       <c r="S193" s="31"/>
     </row>
     <row r="194" spans="4:19">
+      <c r="I194" s="8"/>
       <c r="S194" s="31"/>
     </row>
     <row r="195" spans="4:19">
+      <c r="D195" s="8"/>
       <c r="S195" s="31"/>
     </row>
     <row r="196" spans="4:19">
@@ -21551,17 +21613,9 @@
       <c r="S208" s="31"/>
     </row>
     <row r="209" spans="10:19">
-      <c r="J209"/>
-      <c r="K209"/>
-      <c r="L209"/>
-      <c r="M209"/>
       <c r="S209" s="31"/>
     </row>
     <row r="210" spans="10:19">
-      <c r="J210"/>
-      <c r="K210"/>
-      <c r="L210"/>
-      <c r="M210"/>
       <c r="S210" s="31"/>
     </row>
     <row r="211" spans="10:19">
@@ -25161,6 +25215,20 @@
       <c r="L724"/>
       <c r="M724"/>
       <c r="S724" s="31"/>
+    </row>
+    <row r="725" spans="10:19">
+      <c r="J725"/>
+      <c r="K725"/>
+      <c r="L725"/>
+      <c r="M725"/>
+      <c r="S725" s="31"/>
+    </row>
+    <row r="726" spans="10:19">
+      <c r="J726"/>
+      <c r="K726"/>
+      <c r="L726"/>
+      <c r="M726"/>
+      <c r="S726" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -25175,10 +25243,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4">
       <formula1>$AD$1:$AH$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33:C319 C3:C32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C321">
       <formula1>$AD$2:$AG$2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33:B319 B5:B32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B321">
       <formula1>$AD$1:$AG$1</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>